<commit_message>
Update :: Balance Excel File
1. UpgradeChance Fomula has changed!

upgradeball/(baseball-removeball) (%)
-> (upgradeball+addupgradeball)/(baseball-removeball) (%)
</commit_message>
<xml_diff>
--- a/검 강화 게임.xlsx
+++ b/검 강화 게임.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\문서\GitHub\Unity_Weapon_Forge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EB8F37-7C56-47F8-98E9-65F5957767E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3781DF2E-C12C-4486-856F-02FE3F53BED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8856" xr2:uid="{D3FEDBA6-35E5-45CF-B54A-9F527DCBFA6E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>SELL</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -86,12 +86,23 @@
     <t>-</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddSuccessBall</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +153,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -212,13 +231,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1836,7 +1855,7 @@
             <c:numRef>
               <c:f>Sheet1!$L$4:$L$54</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -1854,142 +1873,142 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.98360655737704916</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.967741935483871</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0.95238095238095233</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.9375</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.92307692307692313</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0.90909090909090906</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>0.89552238805970152</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>0.88235294117647056</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0.86956521739130432</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.9375</c:v>
+                  <c:v>0.8571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.88235294117647056</c:v>
+                  <c:v>0.84507042253521125</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.78947368421052633</c:v>
+                  <c:v>0.82191780821917804</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.75</c:v>
+                  <c:v>0.81081081081081086</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.7142857142857143</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.46875</c:v>
+                  <c:v>0.78947368421052633</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.44117647058823528</c:v>
+                  <c:v>0.77922077922077926</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.41666666666666669</c:v>
+                  <c:v>0.76923076923076927</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.39473684210526316</c:v>
+                  <c:v>0.759493670886076</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.375</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.35714285714285715</c:v>
+                  <c:v>0.7407407407407407</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.34090909090909088</c:v>
+                  <c:v>0.73170731707317072</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.32608695652173914</c:v>
+                  <c:v>0.72289156626506024</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.3125</c:v>
+                  <c:v>0.7142857142857143</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.3</c:v>
+                  <c:v>0.70588235294117652</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.28846153846153844</c:v>
+                  <c:v>0.69767441860465118</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.27777777777777779</c:v>
+                  <c:v>0.68965517241379315</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.26785714285714285</c:v>
+                  <c:v>0.68181818181818177</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.25862068965517243</c:v>
+                  <c:v>0.6741573033707865</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.25</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.24193548387096775</c:v>
+                  <c:v>0.65934065934065933</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.234375</c:v>
+                  <c:v>0.65217391304347827</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.22727272727272727</c:v>
+                  <c:v>0.64516129032258063</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.22058823529411764</c:v>
+                  <c:v>0.63829787234042556</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.16304347826086957</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.15463917525773196</c:v>
+                  <c:v>0.61224489795918369</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.14705882352941177</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.14018691588785046</c:v>
+                  <c:v>0.58823529411764708</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.13392857142857142</c:v>
+                  <c:v>0.57692307692307687</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.12820512820512819</c:v>
+                  <c:v>0.56603773584905659</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.12295081967213115</c:v>
+                  <c:v>0.55555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.11811023622047244</c:v>
+                  <c:v>0.54545454545454541</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.11363636363636363</c:v>
+                  <c:v>0.5357142857142857</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.10948905109489052</c:v>
+                  <c:v>0.52631578947368418</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2084,7 +2103,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3659,8 +3678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62FF258-7648-4ED0-AA06-DFEB56F203C0}">
   <dimension ref="C3:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3706,9 +3725,6 @@
       <c r="N3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O3" t="s">
-        <v>12</v>
-      </c>
       <c r="P3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3739,18 +3755,15 @@
         <v>1000</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K23" si="0">$J4-$O$4</f>
-        <v>200</v>
+        <f t="shared" ref="K4:K23" si="0">$J4-$O$7+$N$7</f>
+        <v>2800</v>
       </c>
       <c r="L4" s="8">
-        <f>IF($N$4&gt;$K4,100%,$N$4/$K4)</f>
+        <f t="shared" ref="L4:L23" si="1">IF($N$4+$N$7&gt;=$K4,100%,($N$4+$N$7)/$K4)</f>
         <v>1</v>
       </c>
       <c r="N4">
-        <v>1500</v>
-      </c>
-      <c r="O4">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="P4">
         <v>1000</v>
@@ -3758,7 +3771,7 @@
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C5" s="2">
-        <f t="shared" ref="C5:C29" si="1">C4+1</f>
+        <f t="shared" ref="C5:C29" si="2">C4+1</f>
         <v>1</v>
       </c>
       <c r="D5" s="1">
@@ -3768,35 +3781,35 @@
         <v>50</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F23" si="2">E5-D4-E4</f>
+        <f t="shared" ref="F5:F23" si="3">E5-D4-E4</f>
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G23" si="3">F5+G4</f>
+        <f t="shared" ref="G5:G23" si="4">F5+G4</f>
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:H23" si="4">F5-F4</f>
+        <f t="shared" ref="H5:H23" si="5">F5-F4</f>
         <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1100</v>
+        <v>1050</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>2850</v>
       </c>
       <c r="L5" s="8">
-        <f>IF($N$4&gt;$K5,100%,$N$4/$K5)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="D6" s="1">
@@ -3806,36 +3819,42 @@
         <v>200</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="G6" s="1">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="H6" s="1">
+      <c r="G6" s="1">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
+      <c r="H6" s="1">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I6:I23" si="5">H6-H5-I5</f>
+        <f t="shared" ref="I6:I23" si="6">H6-H5-I5</f>
         <v>50</v>
       </c>
       <c r="J6">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>2900</v>
       </c>
       <c r="L6" s="8">
-        <f>IF($N$4&gt;$K6,100%,$N$4/$K6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="D7" s="1">
@@ -3845,36 +3864,42 @@
         <v>500</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1300</v>
+        <v>1150</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>2950</v>
       </c>
       <c r="L7" s="8">
-        <f>IF($N$4&gt;$K7,100%,$N$4/$K7)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+      <c r="N7">
+        <v>2000</v>
+      </c>
+      <c r="O7">
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D8" s="1">
@@ -3884,36 +3909,36 @@
         <v>1000</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>500</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="J8">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>3000</v>
       </c>
       <c r="L8" s="8">
-        <f>IF($N$4&gt;$K8,100%,$N$4/$K8)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D9" s="1">
@@ -3923,36 +3948,36 @@
         <v>1800</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>550</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1050</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>250</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="J9">
-        <v>1500</v>
+        <v>1250</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>3050</v>
       </c>
       <c r="L9" s="8">
-        <f>IF($N$4&gt;$K9,100%,$N$4/$K9)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.98360655737704916</v>
       </c>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="D10" s="1">
@@ -3962,36 +3987,36 @@
         <v>3000</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>900</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1950</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>350</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="J10">
-        <v>1600</v>
+        <v>1300</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>3100</v>
       </c>
       <c r="L10" s="8">
-        <f>IF($N$4&gt;$K10,100%,$N$4/$K10)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.967741935483871</v>
       </c>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="D11" s="1">
@@ -4001,36 +4026,36 @@
         <v>4800</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1400</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3350</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>500</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="J11">
-        <v>1700</v>
+        <v>1350</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>3150</v>
       </c>
       <c r="L11" s="8">
-        <f>IF($N$4&gt;$K11,100%,$N$4/$K11)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.95238095238095233</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="D12" s="1">
@@ -4040,36 +4065,36 @@
         <v>7400</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2100</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="3"/>
+        <f>F12+G11</f>
         <v>5450</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>700</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="J12">
-        <v>1800</v>
+        <v>1400</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>3200</v>
       </c>
       <c r="L12" s="8">
-        <f>IF($N$4&gt;$K12,100%,$N$4/$K12)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D13" s="1">
@@ -4079,36 +4104,36 @@
         <v>11050</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3000</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8450</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="J13">
-        <v>1900</v>
+        <v>1450</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>3250</v>
       </c>
       <c r="L13" s="8">
-        <f>IF($N$4&gt;$K13,100%,$N$4/$K13)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.92307692307692313</v>
       </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="D14" s="1">
@@ -4118,36 +4143,36 @@
         <v>16000</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4150</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12600</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1150</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>3300</v>
       </c>
       <c r="L14" s="8">
-        <f>IF($N$4&gt;$K14,100%,$N$4/$K14)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.90909090909090906</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="D15" s="1">
@@ -4157,36 +4182,36 @@
         <v>22600</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5600</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18200</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1450</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="J15">
-        <v>2100</v>
+        <v>1550</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>1300</v>
+        <v>3350</v>
       </c>
       <c r="L15" s="8">
-        <f>IF($N$4&gt;$K15,100%,$N$4/$K15)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.89552238805970152</v>
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="D16" s="1">
@@ -4196,36 +4221,36 @@
         <v>31150</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7350</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25550</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1750</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="J16">
-        <v>2200</v>
+        <v>1600</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>1400</v>
+        <v>3400</v>
       </c>
       <c r="L16" s="8">
-        <f>IF($N$4&gt;$K16,100%,$N$4/$K16)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="D17" s="1">
@@ -4235,36 +4260,36 @@
         <v>42000</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9450</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35000</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2100</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="J17">
-        <v>2300</v>
+        <v>1650</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>3450</v>
       </c>
       <c r="L17" s="8">
-        <f>IF($N$4&gt;$K17,100%,$N$4/$K17)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.86956521739130432</v>
       </c>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="D18" s="1">
@@ -4274,36 +4299,36 @@
         <v>55600</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11950</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46950</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2500</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="J18">
-        <v>2400</v>
+        <v>1700</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>1600</v>
+        <v>3500</v>
       </c>
       <c r="L18" s="8">
-        <f>IF($N$4&gt;$K18,100%,$N$4/$K18)</f>
-        <v>0.9375</v>
+        <f t="shared" si="1"/>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="D19" s="1">
@@ -4313,36 +4338,36 @@
         <v>72350</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14850</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61800</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2900</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="J19">
-        <v>2500</v>
+        <v>1750</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>1700</v>
+        <v>3550</v>
       </c>
       <c r="L19" s="8">
-        <f>IF($N$4&gt;$K19,100%,$N$4/$K19)</f>
-        <v>0.88235294117647056</v>
+        <f t="shared" si="1"/>
+        <v>0.84507042253521125</v>
       </c>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="D20" s="1">
@@ -4352,36 +4377,36 @@
         <v>92750</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18200</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80000</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3350</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>250</v>
       </c>
       <c r="J20">
-        <v>2600</v>
+        <v>1800</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>3600</v>
       </c>
       <c r="L20" s="8">
-        <f>IF($N$4&gt;$K20,100%,$N$4/$K20)</f>
+        <f t="shared" si="1"/>
         <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="D21" s="1">
@@ -4391,36 +4416,36 @@
         <v>117300</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22050</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>102050</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3850</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>250</v>
       </c>
       <c r="J21">
-        <v>2700</v>
+        <v>1850</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>1900</v>
+        <v>3650</v>
       </c>
       <c r="L21" s="8">
-        <f>IF($N$4&gt;$K21,100%,$N$4/$K21)</f>
-        <v>0.78947368421052633</v>
+        <f t="shared" si="1"/>
+        <v>0.82191780821917804</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="D22" s="1">
@@ -4430,36 +4455,36 @@
         <v>146500</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26400</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128450</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4350</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>250</v>
       </c>
       <c r="J22">
-        <v>2800</v>
+        <v>1900</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>3700</v>
       </c>
       <c r="L22" s="8">
-        <f>IF($N$4&gt;$K22,100%,$N$4/$K22)</f>
-        <v>0.75</v>
+        <f t="shared" si="1"/>
+        <v>0.81081081081081086</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="D23" s="1">
@@ -4469,36 +4494,36 @@
         <v>180900</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31300</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>159750</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4900</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="J23">
-        <v>2900</v>
+        <v>1950</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>2100</v>
+        <v>3750</v>
       </c>
       <c r="L23" s="8">
-        <f>IF($N$4&gt;$K23,100%,$N$4/$K23)</f>
-        <v>0.7142857142857143</v>
+        <f t="shared" si="1"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="D24" s="6">
@@ -4519,19 +4544,19 @@
       <c r="I24" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="9">
-        <v>2000</v>
-      </c>
-      <c r="K24" s="9">
-        <v>2000</v>
-      </c>
-      <c r="L24" s="10">
+      <c r="J24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L24" s="9">
         <v>0.7</v>
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="D25" s="1">
@@ -4556,20 +4581,20 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:K54" si="6">$J25-$O$4</f>
-        <v>3200</v>
+        <f t="shared" ref="K25:K43" si="7">$J25-$O$7+$N$7</f>
+        <v>3800</v>
       </c>
       <c r="L25" s="8">
-        <f>IF($N$4&gt;$K25,100%,$N$4/$K25)</f>
-        <v>0.46875</v>
+        <f t="shared" ref="L25:L43" si="8">IF($N$4+$N$7&gt;=$K25,100%,($N$4+$N$7)/$K25)</f>
+        <v>0.78947368421052633</v>
       </c>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="D26" s="1">
@@ -4579,11 +4604,11 @@
         <v>292000</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" ref="F26:F43" si="7">E26-D25-E25</f>
+        <f t="shared" ref="F26:F43" si="9">E26-D25-E25</f>
         <v>37000</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" ref="G26:G43" si="8">F26+G25</f>
+        <f t="shared" ref="G26:G43" si="10">F26+G25</f>
         <v>262450</v>
       </c>
       <c r="H26" s="1">
@@ -4595,20 +4620,20 @@
         <v>500</v>
       </c>
       <c r="J26">
-        <v>4200</v>
+        <v>2050</v>
       </c>
       <c r="K26">
-        <f t="shared" si="6"/>
-        <v>3400</v>
+        <f t="shared" si="7"/>
+        <v>3850</v>
       </c>
       <c r="L26" s="8">
-        <f>IF($N$4&gt;$K26,100%,$N$4/$K26)</f>
-        <v>0.44117647058823528</v>
+        <f t="shared" si="8"/>
+        <v>0.77922077922077926</v>
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="D27" s="1">
@@ -4618,36 +4643,36 @@
         <v>341200</v>
       </c>
       <c r="F27" s="1">
+        <f t="shared" si="9"/>
+        <v>43700</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="10"/>
+        <v>306150</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" ref="H27:H43" si="11">F27-F26</f>
+        <v>6700</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" ref="I27:I43" si="12">H27-H26-I26</f>
+        <v>500</v>
+      </c>
+      <c r="J27">
+        <v>2100</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="7"/>
-        <v>43700</v>
-      </c>
-      <c r="G27" s="1">
+        <v>3900</v>
+      </c>
+      <c r="L27" s="8">
         <f t="shared" si="8"/>
-        <v>306150</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" ref="H27:H43" si="9">F27-F26</f>
-        <v>6700</v>
-      </c>
-      <c r="I27" s="1">
-        <f t="shared" ref="I27:I43" si="10">H27-H26-I26</f>
-        <v>500</v>
-      </c>
-      <c r="J27">
-        <v>4400</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="6"/>
-        <v>3600</v>
-      </c>
-      <c r="L27" s="8">
-        <f>IF($N$4&gt;$K27,100%,$N$4/$K27)</f>
-        <v>0.41666666666666669</v>
+        <v>0.76923076923076927</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="D28" s="1">
@@ -4657,36 +4682,36 @@
         <v>398600</v>
       </c>
       <c r="F28" s="1">
+        <f t="shared" si="9"/>
+        <v>51400</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="10"/>
+        <v>357550</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="11"/>
+        <v>7700</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="12"/>
+        <v>500</v>
+      </c>
+      <c r="J28">
+        <v>2150</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="7"/>
-        <v>51400</v>
-      </c>
-      <c r="G28" s="1">
+        <v>3950</v>
+      </c>
+      <c r="L28" s="8">
         <f t="shared" si="8"/>
-        <v>357550</v>
-      </c>
-      <c r="H28" s="1">
-        <f t="shared" si="9"/>
-        <v>7700</v>
-      </c>
-      <c r="I28" s="1">
-        <f t="shared" si="10"/>
-        <v>500</v>
-      </c>
-      <c r="J28">
-        <v>4600</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="6"/>
-        <v>3800</v>
-      </c>
-      <c r="L28" s="8">
-        <f>IF($N$4&gt;$K28,100%,$N$4/$K28)</f>
-        <v>0.39473684210526316</v>
+        <v>0.759493670886076</v>
       </c>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="D29" s="1">
@@ -4696,36 +4721,36 @@
         <v>465300</v>
       </c>
       <c r="F29" s="1">
+        <f t="shared" si="9"/>
+        <v>60200</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="10"/>
+        <v>417750</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="11"/>
+        <v>8800</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="12"/>
+        <v>600</v>
+      </c>
+      <c r="J29">
+        <v>2200</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="7"/>
-        <v>60200</v>
-      </c>
-      <c r="G29" s="1">
+        <v>4000</v>
+      </c>
+      <c r="L29" s="8">
         <f t="shared" si="8"/>
-        <v>417750</v>
-      </c>
-      <c r="H29" s="1">
-        <f t="shared" si="9"/>
-        <v>8800</v>
-      </c>
-      <c r="I29" s="1">
-        <f t="shared" si="10"/>
-        <v>600</v>
-      </c>
-      <c r="J29">
-        <v>4800</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="6"/>
-        <v>4000</v>
-      </c>
-      <c r="L29" s="8">
-        <f>IF($N$4&gt;$K29,100%,$N$4/$K29)</f>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C30" s="2">
-        <f t="shared" ref="C30:C54" si="11">C29+1</f>
+        <f t="shared" ref="C30:C54" si="13">C29+1</f>
         <v>26</v>
       </c>
       <c r="D30" s="1">
@@ -4735,36 +4760,36 @@
         <v>542500</v>
       </c>
       <c r="F30" s="1">
+        <f t="shared" si="9"/>
+        <v>70200</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="10"/>
+        <v>487950</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="11"/>
+        <v>10000</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="12"/>
+        <v>600</v>
+      </c>
+      <c r="J30">
+        <v>2250</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="7"/>
-        <v>70200</v>
-      </c>
-      <c r="G30" s="1">
+        <v>4050</v>
+      </c>
+      <c r="L30" s="8">
         <f t="shared" si="8"/>
-        <v>487950</v>
-      </c>
-      <c r="H30" s="1">
-        <f t="shared" si="9"/>
-        <v>10000</v>
-      </c>
-      <c r="I30" s="1">
-        <f t="shared" si="10"/>
-        <v>600</v>
-      </c>
-      <c r="J30">
-        <v>5000</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="6"/>
-        <v>4200</v>
-      </c>
-      <c r="L30" s="8">
-        <f>IF($N$4&gt;$K30,100%,$N$4/$K30)</f>
-        <v>0.35714285714285715</v>
+        <v>0.7407407407407407</v>
       </c>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C31" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="D31" s="1">
@@ -4774,36 +4799,36 @@
         <v>631600</v>
       </c>
       <c r="F31" s="1">
+        <f t="shared" si="9"/>
+        <v>81400</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="10"/>
+        <v>569350</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="11"/>
+        <v>11200</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="12"/>
+        <v>600</v>
+      </c>
+      <c r="J31">
+        <v>2300</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="7"/>
-        <v>81400</v>
-      </c>
-      <c r="G31" s="1">
+        <v>4100</v>
+      </c>
+      <c r="L31" s="8">
         <f t="shared" si="8"/>
-        <v>569350</v>
-      </c>
-      <c r="H31" s="1">
-        <f t="shared" si="9"/>
-        <v>11200</v>
-      </c>
-      <c r="I31" s="1">
-        <f t="shared" si="10"/>
-        <v>600</v>
-      </c>
-      <c r="J31">
-        <v>5200</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="6"/>
-        <v>4400</v>
-      </c>
-      <c r="L31" s="8">
-        <f>IF($N$4&gt;$K31,100%,$N$4/$K31)</f>
-        <v>0.34090909090909088</v>
+        <v>0.73170731707317072</v>
       </c>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C32" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="D32" s="1">
@@ -4813,36 +4838,36 @@
         <v>733900</v>
       </c>
       <c r="F32" s="1">
+        <f t="shared" si="9"/>
+        <v>93900</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="10"/>
+        <v>663250</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="11"/>
+        <v>12500</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="12"/>
+        <v>700</v>
+      </c>
+      <c r="J32">
+        <v>2350</v>
+      </c>
+      <c r="K32">
         <f t="shared" si="7"/>
-        <v>93900</v>
-      </c>
-      <c r="G32" s="1">
+        <v>4150</v>
+      </c>
+      <c r="L32" s="8">
         <f t="shared" si="8"/>
-        <v>663250</v>
-      </c>
-      <c r="H32" s="1">
-        <f t="shared" si="9"/>
-        <v>12500</v>
-      </c>
-      <c r="I32" s="1">
-        <f t="shared" si="10"/>
-        <v>700</v>
-      </c>
-      <c r="J32">
-        <v>5400</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="6"/>
-        <v>4600</v>
-      </c>
-      <c r="L32" s="8">
-        <f>IF($N$4&gt;$K32,100%,$N$4/$K32)</f>
-        <v>0.32608695652173914</v>
+        <v>0.72289156626506024</v>
       </c>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C33" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="D33" s="1">
@@ -4852,36 +4877,36 @@
         <v>850900</v>
       </c>
       <c r="F33" s="1">
+        <f t="shared" si="9"/>
+        <v>107800</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="10"/>
+        <v>771050</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="11"/>
+        <v>13900</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="12"/>
+        <v>700</v>
+      </c>
+      <c r="J33">
+        <v>2400</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="7"/>
-        <v>107800</v>
-      </c>
-      <c r="G33" s="1">
+        <v>4200</v>
+      </c>
+      <c r="L33" s="8">
         <f t="shared" si="8"/>
-        <v>771050</v>
-      </c>
-      <c r="H33" s="1">
-        <f t="shared" si="9"/>
-        <v>13900</v>
-      </c>
-      <c r="I33" s="1">
-        <f t="shared" si="10"/>
-        <v>700</v>
-      </c>
-      <c r="J33">
-        <v>5600</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="6"/>
-        <v>4800</v>
-      </c>
-      <c r="L33" s="8">
-        <f>IF($N$4&gt;$K33,100%,$N$4/$K33)</f>
-        <v>0.3125</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C34" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
       <c r="D34" s="1">
@@ -4891,36 +4916,36 @@
         <v>984000</v>
       </c>
       <c r="F34" s="1">
+        <f t="shared" si="9"/>
+        <v>123100</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="10"/>
+        <v>894150</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="11"/>
+        <v>15300</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="12"/>
+        <v>700</v>
+      </c>
+      <c r="J34">
+        <v>2450</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="7"/>
-        <v>123100</v>
-      </c>
-      <c r="G34" s="1">
+        <v>4250</v>
+      </c>
+      <c r="L34" s="8">
         <f t="shared" si="8"/>
-        <v>894150</v>
-      </c>
-      <c r="H34" s="1">
-        <f t="shared" si="9"/>
-        <v>15300</v>
-      </c>
-      <c r="I34" s="1">
-        <f t="shared" si="10"/>
-        <v>700</v>
-      </c>
-      <c r="J34">
-        <v>5800</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="6"/>
-        <v>5000</v>
-      </c>
-      <c r="L34" s="8">
-        <f>IF($N$4&gt;$K34,100%,$N$4/$K34)</f>
-        <v>0.3</v>
+        <v>0.70588235294117652</v>
       </c>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C35" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31</v>
       </c>
       <c r="D35" s="1">
@@ -4930,36 +4955,36 @@
         <v>1134700</v>
       </c>
       <c r="F35" s="1">
+        <f t="shared" si="9"/>
+        <v>139900</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="10"/>
+        <v>1034050</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="11"/>
+        <v>16800</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="12"/>
+        <v>800</v>
+      </c>
+      <c r="J35">
+        <v>2500</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="7"/>
-        <v>139900</v>
-      </c>
-      <c r="G35" s="1">
+        <v>4300</v>
+      </c>
+      <c r="L35" s="8">
         <f t="shared" si="8"/>
-        <v>1034050</v>
-      </c>
-      <c r="H35" s="1">
-        <f t="shared" si="9"/>
-        <v>16800</v>
-      </c>
-      <c r="I35" s="1">
-        <f t="shared" si="10"/>
-        <v>800</v>
-      </c>
-      <c r="J35">
-        <v>6000</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="6"/>
-        <v>5200</v>
-      </c>
-      <c r="L35" s="8">
-        <f>IF($N$4&gt;$K35,100%,$N$4/$K35)</f>
-        <v>0.28846153846153844</v>
+        <v>0.69767441860465118</v>
       </c>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C36" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>32</v>
       </c>
       <c r="D36" s="1">
@@ -4969,36 +4994,36 @@
         <v>1304600</v>
       </c>
       <c r="F36" s="1">
+        <f t="shared" si="9"/>
+        <v>158300</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="10"/>
+        <v>1192350</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="11"/>
+        <v>18400</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="12"/>
+        <v>800</v>
+      </c>
+      <c r="J36">
+        <v>2550</v>
+      </c>
+      <c r="K36">
         <f t="shared" si="7"/>
-        <v>158300</v>
-      </c>
-      <c r="G36" s="1">
+        <v>4350</v>
+      </c>
+      <c r="L36" s="8">
         <f t="shared" si="8"/>
-        <v>1192350</v>
-      </c>
-      <c r="H36" s="1">
-        <f t="shared" si="9"/>
-        <v>18400</v>
-      </c>
-      <c r="I36" s="1">
-        <f t="shared" si="10"/>
-        <v>800</v>
-      </c>
-      <c r="J36">
-        <v>6200</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="6"/>
-        <v>5400</v>
-      </c>
-      <c r="L36" s="8">
-        <f>IF($N$4&gt;$K36,100%,$N$4/$K36)</f>
-        <v>0.27777777777777779</v>
+        <v>0.68965517241379315</v>
       </c>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C37" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>33</v>
       </c>
       <c r="D37" s="1">
@@ -5008,36 +5033,36 @@
         <v>1495400</v>
       </c>
       <c r="F37" s="1">
+        <f t="shared" si="9"/>
+        <v>178300</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="10"/>
+        <v>1370650</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="11"/>
+        <v>20000</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="12"/>
+        <v>800</v>
+      </c>
+      <c r="J37">
+        <v>2600</v>
+      </c>
+      <c r="K37">
         <f t="shared" si="7"/>
-        <v>178300</v>
-      </c>
-      <c r="G37" s="1">
+        <v>4400</v>
+      </c>
+      <c r="L37" s="8">
         <f t="shared" si="8"/>
-        <v>1370650</v>
-      </c>
-      <c r="H37" s="1">
-        <f t="shared" si="9"/>
-        <v>20000</v>
-      </c>
-      <c r="I37" s="1">
-        <f t="shared" si="10"/>
-        <v>800</v>
-      </c>
-      <c r="J37">
-        <v>6400</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="6"/>
-        <v>5600</v>
-      </c>
-      <c r="L37" s="8">
-        <f>IF($N$4&gt;$K37,100%,$N$4/$K37)</f>
-        <v>0.26785714285714285</v>
+        <v>0.68181818181818177</v>
       </c>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C38" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
       <c r="D38" s="1">
@@ -5047,36 +5072,36 @@
         <v>1708800</v>
       </c>
       <c r="F38" s="1">
+        <f t="shared" si="9"/>
+        <v>200000</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="10"/>
+        <v>1570650</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="11"/>
+        <v>21700</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="12"/>
+        <v>900</v>
+      </c>
+      <c r="J38">
+        <v>2650</v>
+      </c>
+      <c r="K38">
         <f t="shared" si="7"/>
-        <v>200000</v>
-      </c>
-      <c r="G38" s="1">
+        <v>4450</v>
+      </c>
+      <c r="L38" s="8">
         <f t="shared" si="8"/>
-        <v>1570650</v>
-      </c>
-      <c r="H38" s="1">
-        <f t="shared" si="9"/>
-        <v>21700</v>
-      </c>
-      <c r="I38" s="1">
-        <f t="shared" si="10"/>
-        <v>900</v>
-      </c>
-      <c r="J38">
-        <v>6600</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="6"/>
-        <v>5800</v>
-      </c>
-      <c r="L38" s="8">
-        <f>IF($N$4&gt;$K38,100%,$N$4/$K38)</f>
-        <v>0.25862068965517243</v>
+        <v>0.6741573033707865</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C39" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>35</v>
       </c>
       <c r="D39" s="1">
@@ -5086,36 +5111,36 @@
         <v>1946600</v>
       </c>
       <c r="F39" s="1">
+        <f t="shared" si="9"/>
+        <v>223500</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="10"/>
+        <v>1794150</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="11"/>
+        <v>23500</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="12"/>
+        <v>900</v>
+      </c>
+      <c r="J39">
+        <v>2700</v>
+      </c>
+      <c r="K39">
         <f t="shared" si="7"/>
-        <v>223500</v>
-      </c>
-      <c r="G39" s="1">
+        <v>4500</v>
+      </c>
+      <c r="L39" s="8">
         <f t="shared" si="8"/>
-        <v>1794150</v>
-      </c>
-      <c r="H39" s="1">
-        <f t="shared" si="9"/>
-        <v>23500</v>
-      </c>
-      <c r="I39" s="1">
-        <f t="shared" si="10"/>
-        <v>900</v>
-      </c>
-      <c r="J39">
-        <v>6800</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="6"/>
-        <v>6000</v>
-      </c>
-      <c r="L39" s="8">
-        <f>IF($N$4&gt;$K39,100%,$N$4/$K39)</f>
-        <v>0.25</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C40" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
       <c r="D40" s="1">
@@ -5125,36 +5150,36 @@
         <v>2210700</v>
       </c>
       <c r="F40" s="1">
+        <f t="shared" si="9"/>
+        <v>248800</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="10"/>
+        <v>2042950</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="11"/>
+        <v>25300</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="12"/>
+        <v>900</v>
+      </c>
+      <c r="J40">
+        <v>2750</v>
+      </c>
+      <c r="K40">
         <f t="shared" si="7"/>
-        <v>248800</v>
-      </c>
-      <c r="G40" s="1">
+        <v>4550</v>
+      </c>
+      <c r="L40" s="8">
         <f t="shared" si="8"/>
-        <v>2042950</v>
-      </c>
-      <c r="H40" s="1">
-        <f t="shared" si="9"/>
-        <v>25300</v>
-      </c>
-      <c r="I40" s="1">
-        <f t="shared" si="10"/>
-        <v>900</v>
-      </c>
-      <c r="J40">
-        <v>7000</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="6"/>
-        <v>6200</v>
-      </c>
-      <c r="L40" s="8">
-        <f>IF($N$4&gt;$K40,100%,$N$4/$K40)</f>
-        <v>0.24193548387096775</v>
+        <v>0.65934065934065933</v>
       </c>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C41" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="D41" s="1">
@@ -5164,36 +5189,36 @@
         <v>2503000</v>
       </c>
       <c r="F41" s="1">
+        <f t="shared" si="9"/>
+        <v>276000</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="10"/>
+        <v>2318950</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="11"/>
+        <v>27200</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="J41">
+        <v>2800</v>
+      </c>
+      <c r="K41">
         <f t="shared" si="7"/>
-        <v>276000</v>
-      </c>
-      <c r="G41" s="1">
+        <v>4600</v>
+      </c>
+      <c r="L41" s="8">
         <f t="shared" si="8"/>
-        <v>2318950</v>
-      </c>
-      <c r="H41" s="1">
-        <f t="shared" si="9"/>
-        <v>27200</v>
-      </c>
-      <c r="I41" s="1">
-        <f t="shared" si="10"/>
-        <v>1000</v>
-      </c>
-      <c r="J41">
-        <v>7200</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="6"/>
-        <v>6400</v>
-      </c>
-      <c r="L41" s="8">
-        <f>IF($N$4&gt;$K41,100%,$N$4/$K41)</f>
-        <v>0.234375</v>
+        <v>0.65217391304347827</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C42" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>38</v>
       </c>
       <c r="D42" s="1">
@@ -5203,36 +5228,36 @@
         <v>2825500</v>
       </c>
       <c r="F42" s="1">
+        <f t="shared" si="9"/>
+        <v>305200</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="10"/>
+        <v>2624150</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="11"/>
+        <v>29200</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="J42">
+        <v>2850</v>
+      </c>
+      <c r="K42">
         <f t="shared" si="7"/>
-        <v>305200</v>
-      </c>
-      <c r="G42" s="1">
+        <v>4650</v>
+      </c>
+      <c r="L42" s="8">
         <f t="shared" si="8"/>
-        <v>2624150</v>
-      </c>
-      <c r="H42" s="1">
-        <f t="shared" si="9"/>
-        <v>29200</v>
-      </c>
-      <c r="I42" s="1">
-        <f t="shared" si="10"/>
-        <v>1000</v>
-      </c>
-      <c r="J42">
-        <v>7400</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="6"/>
-        <v>6600</v>
-      </c>
-      <c r="L42" s="8">
-        <f>IF($N$4&gt;$K42,100%,$N$4/$K42)</f>
-        <v>0.22727272727272727</v>
+        <v>0.64516129032258063</v>
       </c>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C43" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>39</v>
       </c>
       <c r="D43" s="1">
@@ -5242,36 +5267,36 @@
         <v>3180300</v>
       </c>
       <c r="F43" s="1">
+        <f t="shared" si="9"/>
+        <v>336400</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="10"/>
+        <v>2960550</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="11"/>
+        <v>31200</v>
+      </c>
+      <c r="I43" s="1">
+        <f t="shared" si="12"/>
+        <v>1000</v>
+      </c>
+      <c r="J43">
+        <v>2900</v>
+      </c>
+      <c r="K43">
         <f t="shared" si="7"/>
-        <v>336400</v>
-      </c>
-      <c r="G43" s="1">
+        <v>4700</v>
+      </c>
+      <c r="L43" s="8">
         <f t="shared" si="8"/>
-        <v>2960550</v>
-      </c>
-      <c r="H43" s="1">
-        <f t="shared" si="9"/>
-        <v>31200</v>
-      </c>
-      <c r="I43" s="1">
-        <f t="shared" si="10"/>
-        <v>1000</v>
-      </c>
-      <c r="J43">
-        <v>7600</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="6"/>
-        <v>6800</v>
-      </c>
-      <c r="L43" s="8">
-        <f>IF($N$4&gt;$K43,100%,$N$4/$K43)</f>
-        <v>0.22058823529411764</v>
+        <v>0.63829787234042556</v>
       </c>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C44" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>40</v>
       </c>
       <c r="D44" s="6">
@@ -5292,20 +5317,19 @@
       <c r="I44" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J44" s="9">
-        <v>2000</v>
-      </c>
-      <c r="K44" s="9">
-        <f t="shared" si="6"/>
-        <v>1200</v>
-      </c>
-      <c r="L44" s="10">
+      <c r="J44" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L44" s="9">
         <v>0.5</v>
       </c>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C45" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>41</v>
       </c>
       <c r="D45" s="1">
@@ -5330,20 +5354,20 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="K45">
-        <f t="shared" si="6"/>
-        <v>9200</v>
+        <f t="shared" ref="K45:K54" si="14">$J45-$O$7+$N$7</f>
+        <v>4800</v>
       </c>
       <c r="L45" s="8">
-        <f>IF($N$4&gt;$K45,100%,$N$4/$K45)</f>
-        <v>0.16304347826086957</v>
+        <f t="shared" ref="L45:L54" si="15">IF($N$4+$N$7&gt;=$K45,100%,($N$4+$N$7)/$K45)</f>
+        <v>0.625</v>
       </c>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C46" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>42</v>
       </c>
       <c r="D46" s="1">
@@ -5353,11 +5377,11 @@
         <v>4200100</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" ref="F46:F54" si="12">E46-D45-E45</f>
+        <f t="shared" ref="F46:F54" si="16">E46-D45-E45</f>
         <v>370100</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" ref="G46:G54" si="13">F46+G45</f>
+        <f t="shared" ref="G46:G54" si="17">F46+G45</f>
         <v>3930850</v>
       </c>
       <c r="H46" s="1">
@@ -5369,20 +5393,20 @@
         <v>1500</v>
       </c>
       <c r="J46">
-        <v>10500</v>
+        <v>3100</v>
       </c>
       <c r="K46">
-        <f t="shared" si="6"/>
-        <v>9700</v>
+        <f t="shared" si="14"/>
+        <v>4900</v>
       </c>
       <c r="L46" s="8">
-        <f>IF($N$4&gt;$K46,100%,$N$4/$K46)</f>
-        <v>0.15463917525773196</v>
+        <f t="shared" si="15"/>
+        <v>0.61224489795918369</v>
       </c>
     </row>
     <row r="47" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C47" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>43</v>
       </c>
       <c r="D47" s="1">
@@ -5392,36 +5416,36 @@
         <v>4640000</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>406900</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>4337750</v>
       </c>
       <c r="H47" s="1">
-        <f t="shared" ref="H47:H54" si="14">F47-F46</f>
+        <f t="shared" ref="H47:H54" si="18">F47-F46</f>
         <v>36800</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" ref="I47:I54" si="15">H47-H46-I46</f>
+        <f t="shared" ref="I47:I54" si="19">H47-H46-I46</f>
         <v>1600</v>
       </c>
       <c r="J47">
-        <v>11000</v>
+        <v>3200</v>
       </c>
       <c r="K47">
-        <f t="shared" si="6"/>
-        <v>10200</v>
+        <f t="shared" si="14"/>
+        <v>5000</v>
       </c>
       <c r="L47" s="8">
-        <f>IF($N$4&gt;$K47,100%,$N$4/$K47)</f>
-        <v>0.14705882352941177</v>
+        <f t="shared" si="15"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="48" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C48" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>44</v>
       </c>
       <c r="D48" s="1">
@@ -5431,36 +5455,36 @@
         <v>5123000</v>
       </c>
       <c r="F48" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>447000</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>4784750</v>
       </c>
       <c r="H48" s="1">
+        <f t="shared" si="18"/>
+        <v>40100</v>
+      </c>
+      <c r="I48" s="1">
+        <f t="shared" si="19"/>
+        <v>1700</v>
+      </c>
+      <c r="J48">
+        <v>3300</v>
+      </c>
+      <c r="K48">
         <f t="shared" si="14"/>
-        <v>40100</v>
-      </c>
-      <c r="I48" s="1">
+        <v>5100</v>
+      </c>
+      <c r="L48" s="8">
         <f t="shared" si="15"/>
-        <v>1700</v>
-      </c>
-      <c r="J48">
-        <v>11500</v>
-      </c>
-      <c r="K48">
-        <f t="shared" si="6"/>
-        <v>10700</v>
-      </c>
-      <c r="L48" s="8">
-        <f>IF($N$4&gt;$K48,100%,$N$4/$K48)</f>
-        <v>0.14018691588785046</v>
+        <v>0.58823529411764708</v>
       </c>
     </row>
     <row r="49" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C49" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="D49" s="1">
@@ -5470,36 +5494,36 @@
         <v>5652600</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>490600</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>5275350</v>
       </c>
       <c r="H49" s="1">
+        <f t="shared" si="18"/>
+        <v>43600</v>
+      </c>
+      <c r="I49" s="1">
+        <f t="shared" si="19"/>
+        <v>1800</v>
+      </c>
+      <c r="J49">
+        <v>3400</v>
+      </c>
+      <c r="K49">
         <f t="shared" si="14"/>
-        <v>43600</v>
-      </c>
-      <c r="I49" s="1">
+        <v>5200</v>
+      </c>
+      <c r="L49" s="8">
         <f t="shared" si="15"/>
-        <v>1800</v>
-      </c>
-      <c r="J49">
-        <v>12000</v>
-      </c>
-      <c r="K49">
-        <f t="shared" si="6"/>
-        <v>11200</v>
-      </c>
-      <c r="L49" s="8">
-        <f>IF($N$4&gt;$K49,100%,$N$4/$K49)</f>
-        <v>0.13392857142857142</v>
+        <v>0.57692307692307687</v>
       </c>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C50" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>46</v>
       </c>
       <c r="D50" s="1">
@@ -5509,36 +5533,36 @@
         <v>6232500</v>
       </c>
       <c r="F50" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>537900</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>5813250</v>
       </c>
       <c r="H50" s="1">
+        <f t="shared" si="18"/>
+        <v>47300</v>
+      </c>
+      <c r="I50" s="1">
+        <f t="shared" si="19"/>
+        <v>1900</v>
+      </c>
+      <c r="J50">
+        <v>3500</v>
+      </c>
+      <c r="K50">
         <f t="shared" si="14"/>
-        <v>47300</v>
-      </c>
-      <c r="I50" s="1">
+        <v>5300</v>
+      </c>
+      <c r="L50" s="8">
         <f t="shared" si="15"/>
-        <v>1900</v>
-      </c>
-      <c r="J50">
-        <v>12500</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="6"/>
-        <v>11700</v>
-      </c>
-      <c r="L50" s="8">
-        <f>IF($N$4&gt;$K50,100%,$N$4/$K50)</f>
-        <v>0.12820512820512819</v>
+        <v>0.56603773584905659</v>
       </c>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C51" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>47</v>
       </c>
       <c r="D51" s="1">
@@ -5548,36 +5572,36 @@
         <v>6866600</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>589100</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>6402350</v>
       </c>
       <c r="H51" s="1">
+        <f t="shared" si="18"/>
+        <v>51200</v>
+      </c>
+      <c r="I51" s="1">
+        <f t="shared" si="19"/>
+        <v>2000</v>
+      </c>
+      <c r="J51">
+        <v>3600</v>
+      </c>
+      <c r="K51">
         <f t="shared" si="14"/>
-        <v>51200</v>
-      </c>
-      <c r="I51" s="1">
+        <v>5400</v>
+      </c>
+      <c r="L51" s="8">
         <f t="shared" si="15"/>
-        <v>2000</v>
-      </c>
-      <c r="J51">
-        <v>13000</v>
-      </c>
-      <c r="K51">
-        <f t="shared" si="6"/>
-        <v>12200</v>
-      </c>
-      <c r="L51" s="8">
-        <f>IF($N$4&gt;$K51,100%,$N$4/$K51)</f>
-        <v>0.12295081967213115</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C52" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>48</v>
       </c>
       <c r="D52" s="1">
@@ -5587,36 +5611,36 @@
         <v>7561000</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>644400</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>7046750</v>
       </c>
       <c r="H52" s="1">
+        <f t="shared" si="18"/>
+        <v>55300</v>
+      </c>
+      <c r="I52" s="1">
+        <f t="shared" si="19"/>
+        <v>2100</v>
+      </c>
+      <c r="J52">
+        <v>3700</v>
+      </c>
+      <c r="K52">
         <f t="shared" si="14"/>
-        <v>55300</v>
-      </c>
-      <c r="I52" s="1">
+        <v>5500</v>
+      </c>
+      <c r="L52" s="8">
         <f t="shared" si="15"/>
-        <v>2100</v>
-      </c>
-      <c r="J52">
-        <v>13500</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="6"/>
-        <v>12700</v>
-      </c>
-      <c r="L52" s="8">
-        <f>IF($N$4&gt;$K52,100%,$N$4/$K52)</f>
-        <v>0.11811023622047244</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C53" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="D53" s="1">
@@ -5626,36 +5650,36 @@
         <v>8320000</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>704000</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>7750750</v>
       </c>
       <c r="H53" s="1">
+        <f t="shared" si="18"/>
+        <v>59600</v>
+      </c>
+      <c r="I53" s="1">
+        <f t="shared" si="19"/>
+        <v>2200</v>
+      </c>
+      <c r="J53">
+        <v>3800</v>
+      </c>
+      <c r="K53">
         <f t="shared" si="14"/>
-        <v>59600</v>
-      </c>
-      <c r="I53" s="1">
+        <v>5600</v>
+      </c>
+      <c r="L53" s="8">
         <f t="shared" si="15"/>
-        <v>2200</v>
-      </c>
-      <c r="J53">
-        <v>14000</v>
-      </c>
-      <c r="K53">
-        <f t="shared" si="6"/>
-        <v>13200</v>
-      </c>
-      <c r="L53" s="8">
-        <f>IF($N$4&gt;$K53,100%,$N$4/$K53)</f>
-        <v>0.11363636363636363</v>
+        <v>0.5357142857142857</v>
       </c>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.4">
       <c r="C54" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="D54" s="1">
@@ -5665,31 +5689,31 @@
         <v>9148100</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>768100</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>8518850</v>
       </c>
       <c r="H54" s="1">
+        <f t="shared" si="18"/>
+        <v>64100</v>
+      </c>
+      <c r="I54" s="1">
+        <f t="shared" si="19"/>
+        <v>2300</v>
+      </c>
+      <c r="J54">
+        <v>3900</v>
+      </c>
+      <c r="K54">
         <f t="shared" si="14"/>
-        <v>64100</v>
-      </c>
-      <c r="I54" s="1">
+        <v>5700</v>
+      </c>
+      <c r="L54" s="8">
         <f t="shared" si="15"/>
-        <v>2300</v>
-      </c>
-      <c r="J54">
-        <v>14500</v>
-      </c>
-      <c r="K54">
-        <f t="shared" si="6"/>
-        <v>13700</v>
-      </c>
-      <c r="L54" s="8">
-        <f>IF($N$4&gt;$K54,100%,$N$4/$K54)</f>
-        <v>0.10948905109489052</v>
+        <v>0.52631578947368418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIXED :: Excel File
BaseBall is now more less!
</commit_message>
<xml_diff>
--- a/검 강화 게임.xlsx
+++ b/검 강화 게임.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\문서\GitHub\Unity_Weapon_Forge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3781DF2E-C12C-4486-856F-02FE3F53BED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F172C19-E398-4D40-B657-D498C1F5FF75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8856" xr2:uid="{D3FEDBA6-35E5-45CF-B54A-9F527DCBFA6E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>SELL</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -92,6 +92,14 @@
   </si>
   <si>
     <t>AddSuccessBall</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASBlevel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RBlevel</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1873,142 +1881,142 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98360655737704916</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.967741935483871</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.95238095238095233</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.9375</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.92307692307692313</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.90909090909090906</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.89552238805970152</c:v>
+                  <c:v>0.86956521739130432</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.88235294117647056</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.86956521739130432</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.8571428571428571</c:v>
+                  <c:v>0.76923076923076927</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.84507042253521125</c:v>
+                  <c:v>0.7407407407407407</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>0.7142857142857143</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.82191780821917804</c:v>
+                  <c:v>0.68965517241379315</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.81081081081081086</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.8</c:v>
+                  <c:v>0.64516129032258063</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.78947368421052633</c:v>
+                  <c:v>0.60606060606060608</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.77922077922077926</c:v>
+                  <c:v>0.58823529411764708</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.76923076923076927</c:v>
+                  <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.759493670886076</c:v>
+                  <c:v>0.55555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.75</c:v>
+                  <c:v>0.54054054054054057</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.7407407407407407</c:v>
+                  <c:v>0.52631578947368418</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.73170731707317072</c:v>
+                  <c:v>0.51282051282051277</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.72289156626506024</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.7142857142857143</c:v>
+                  <c:v>0.48780487804878048</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.70588235294117652</c:v>
+                  <c:v>0.47619047619047616</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.69767441860465118</c:v>
+                  <c:v>0.46511627906976744</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.68965517241379315</c:v>
+                  <c:v>0.45454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.68181818181818177</c:v>
+                  <c:v>0.44444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.6741573033707865</c:v>
+                  <c:v>0.43478260869565216</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.42553191489361702</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.65934065934065933</c:v>
+                  <c:v>0.41666666666666669</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.65217391304347827</c:v>
+                  <c:v>0.40816326530612246</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.64516129032258063</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.63829787234042556</c:v>
+                  <c:v>0.39215686274509803</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.625</c:v>
+                  <c:v>0.37037037037037035</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.61224489795918369</c:v>
+                  <c:v>0.35714285714285715</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.6</c:v>
+                  <c:v>0.34482758620689657</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.58823529411764708</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.57692307692307687</c:v>
+                  <c:v>0.32258064516129031</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.56603773584905659</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.55555555555555558</c:v>
+                  <c:v>0.30303030303030304</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.54545454545454541</c:v>
+                  <c:v>0.29411764705882354</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.5357142857142857</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.52631578947368418</c:v>
+                  <c:v>0.27777777777777779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3678,8 +3686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62FF258-7648-4ED0-AA06-DFEB56F203C0}">
   <dimension ref="C3:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="57" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3752,18 +3760,18 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K23" si="0">$J4-$O$7+$N$7</f>
-        <v>2800</v>
+        <v>120</v>
       </c>
       <c r="L4" s="8">
         <f t="shared" ref="L4:L23" si="1">IF($N$4+$N$7&gt;=$K4,100%,($N$4+$N$7)/$K4)</f>
         <v>1</v>
       </c>
       <c r="N4">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="P4">
         <v>1000</v>
@@ -3796,11 +3804,11 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1050</v>
+        <v>210</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>2850</v>
+        <v>130</v>
       </c>
       <c r="L5" s="8">
         <f t="shared" si="1"/>
@@ -3835,11 +3843,11 @@
         <v>50</v>
       </c>
       <c r="J6">
-        <v>1100</v>
+        <v>220</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>2900</v>
+        <v>140</v>
       </c>
       <c r="L6" s="8">
         <f t="shared" si="1"/>
@@ -3880,21 +3888,23 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1150</v>
+        <v>230</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>2950</v>
+        <v>150</v>
       </c>
       <c r="L7" s="8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N7">
-        <v>2000</v>
+        <f>$N$11*32</f>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>200</v>
+        <f>$O$11*16</f>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.4">
@@ -3925,11 +3935,11 @@
         <v>50</v>
       </c>
       <c r="J8">
-        <v>1200</v>
+        <v>240</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>160</v>
       </c>
       <c r="L8" s="8">
         <f t="shared" si="1"/>
@@ -3964,15 +3974,15 @@
         <v>50</v>
       </c>
       <c r="J9">
-        <v>1250</v>
+        <v>250</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>3050</v>
+        <v>170</v>
       </c>
       <c r="L9" s="8">
         <f t="shared" si="1"/>
-        <v>0.98360655737704916</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.4">
@@ -4003,15 +4013,21 @@
         <v>50</v>
       </c>
       <c r="J10">
-        <v>1300</v>
+        <v>260</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>180</v>
       </c>
       <c r="L10" s="8">
         <f t="shared" si="1"/>
-        <v>0.967741935483871</v>
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.4">
@@ -4042,15 +4058,21 @@
         <v>100</v>
       </c>
       <c r="J11">
-        <v>1350</v>
+        <v>270</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>3150</v>
+        <v>190</v>
       </c>
       <c r="L11" s="8">
         <f t="shared" si="1"/>
-        <v>0.95238095238095233</v>
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.4">
@@ -4081,15 +4103,15 @@
         <v>100</v>
       </c>
       <c r="J12">
-        <v>1400</v>
+        <v>280</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>3200</v>
+        <v>200</v>
       </c>
       <c r="L12" s="8">
         <f t="shared" si="1"/>
-        <v>0.9375</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.4">
@@ -4120,15 +4142,15 @@
         <v>100</v>
       </c>
       <c r="J13">
-        <v>1450</v>
+        <v>290</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>3250</v>
+        <v>210</v>
       </c>
       <c r="L13" s="8">
         <f t="shared" si="1"/>
-        <v>0.92307692307692313</v>
+        <v>0.95238095238095233</v>
       </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.4">
@@ -4159,11 +4181,11 @@
         <v>150</v>
       </c>
       <c r="J14">
-        <v>1500</v>
+        <v>300</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>3300</v>
+        <v>220</v>
       </c>
       <c r="L14" s="8">
         <f t="shared" si="1"/>
@@ -4198,15 +4220,15 @@
         <v>150</v>
       </c>
       <c r="J15">
-        <v>1550</v>
+        <v>310</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>3350</v>
+        <v>230</v>
       </c>
       <c r="L15" s="8">
         <f t="shared" si="1"/>
-        <v>0.89552238805970152</v>
+        <v>0.86956521739130432</v>
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.4">
@@ -4237,15 +4259,15 @@
         <v>150</v>
       </c>
       <c r="J16">
-        <v>1600</v>
+        <v>320</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>3400</v>
+        <v>240</v>
       </c>
       <c r="L16" s="8">
         <f t="shared" si="1"/>
-        <v>0.88235294117647056</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.4">
@@ -4276,15 +4298,15 @@
         <v>200</v>
       </c>
       <c r="J17">
-        <v>1650</v>
+        <v>330</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>3450</v>
+        <v>250</v>
       </c>
       <c r="L17" s="8">
         <f t="shared" si="1"/>
-        <v>0.86956521739130432</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.4">
@@ -4315,15 +4337,15 @@
         <v>200</v>
       </c>
       <c r="J18">
-        <v>1700</v>
+        <v>340</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>3500</v>
+        <v>260</v>
       </c>
       <c r="L18" s="8">
         <f t="shared" si="1"/>
-        <v>0.8571428571428571</v>
+        <v>0.76923076923076927</v>
       </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.4">
@@ -4354,15 +4376,15 @@
         <v>200</v>
       </c>
       <c r="J19">
-        <v>1750</v>
+        <v>350</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>3550</v>
+        <v>270</v>
       </c>
       <c r="L19" s="8">
         <f t="shared" si="1"/>
-        <v>0.84507042253521125</v>
+        <v>0.7407407407407407</v>
       </c>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.4">
@@ -4393,15 +4415,15 @@
         <v>250</v>
       </c>
       <c r="J20">
-        <v>1800</v>
+        <v>360</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>280</v>
       </c>
       <c r="L20" s="8">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.4">
@@ -4432,15 +4454,15 @@
         <v>250</v>
       </c>
       <c r="J21">
-        <v>1850</v>
+        <v>370</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>3650</v>
+        <v>290</v>
       </c>
       <c r="L21" s="8">
         <f t="shared" si="1"/>
-        <v>0.82191780821917804</v>
+        <v>0.68965517241379315</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.4">
@@ -4471,15 +4493,15 @@
         <v>250</v>
       </c>
       <c r="J22">
-        <v>1900</v>
+        <v>380</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>3700</v>
+        <v>300</v>
       </c>
       <c r="L22" s="8">
         <f t="shared" si="1"/>
-        <v>0.81081081081081086</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.4">
@@ -4510,15 +4532,15 @@
         <v>300</v>
       </c>
       <c r="J23">
-        <v>1950</v>
+        <v>390</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>3750</v>
+        <v>310</v>
       </c>
       <c r="L23" s="8">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.64516129032258063</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.4">
@@ -4581,15 +4603,15 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>2000</v>
+        <v>410</v>
       </c>
       <c r="K25">
         <f t="shared" ref="K25:K43" si="7">$J25-$O$7+$N$7</f>
-        <v>3800</v>
+        <v>330</v>
       </c>
       <c r="L25" s="8">
         <f t="shared" ref="L25:L43" si="8">IF($N$4+$N$7&gt;=$K25,100%,($N$4+$N$7)/$K25)</f>
-        <v>0.78947368421052633</v>
+        <v>0.60606060606060608</v>
       </c>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.4">
@@ -4620,15 +4642,15 @@
         <v>500</v>
       </c>
       <c r="J26">
-        <v>2050</v>
+        <v>420</v>
       </c>
       <c r="K26">
         <f t="shared" si="7"/>
-        <v>3850</v>
+        <v>340</v>
       </c>
       <c r="L26" s="8">
         <f t="shared" si="8"/>
-        <v>0.77922077922077926</v>
+        <v>0.58823529411764708</v>
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.4">
@@ -4659,15 +4681,15 @@
         <v>500</v>
       </c>
       <c r="J27">
-        <v>2100</v>
+        <v>430</v>
       </c>
       <c r="K27">
         <f t="shared" si="7"/>
-        <v>3900</v>
+        <v>350</v>
       </c>
       <c r="L27" s="8">
         <f t="shared" si="8"/>
-        <v>0.76923076923076927</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.4">
@@ -4698,15 +4720,15 @@
         <v>500</v>
       </c>
       <c r="J28">
-        <v>2150</v>
+        <v>440</v>
       </c>
       <c r="K28">
         <f t="shared" si="7"/>
-        <v>3950</v>
+        <v>360</v>
       </c>
       <c r="L28" s="8">
         <f t="shared" si="8"/>
-        <v>0.759493670886076</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.4">
@@ -4737,15 +4759,15 @@
         <v>600</v>
       </c>
       <c r="J29">
-        <v>2200</v>
+        <v>450</v>
       </c>
       <c r="K29">
         <f t="shared" si="7"/>
-        <v>4000</v>
+        <v>370</v>
       </c>
       <c r="L29" s="8">
         <f t="shared" si="8"/>
-        <v>0.75</v>
+        <v>0.54054054054054057</v>
       </c>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.4">
@@ -4776,15 +4798,15 @@
         <v>600</v>
       </c>
       <c r="J30">
-        <v>2250</v>
+        <v>460</v>
       </c>
       <c r="K30">
         <f t="shared" si="7"/>
-        <v>4050</v>
+        <v>380</v>
       </c>
       <c r="L30" s="8">
         <f t="shared" si="8"/>
-        <v>0.7407407407407407</v>
+        <v>0.52631578947368418</v>
       </c>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.4">
@@ -4815,15 +4837,15 @@
         <v>600</v>
       </c>
       <c r="J31">
-        <v>2300</v>
+        <v>470</v>
       </c>
       <c r="K31">
         <f t="shared" si="7"/>
-        <v>4100</v>
+        <v>390</v>
       </c>
       <c r="L31" s="8">
         <f t="shared" si="8"/>
-        <v>0.73170731707317072</v>
+        <v>0.51282051282051277</v>
       </c>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.4">
@@ -4854,15 +4876,15 @@
         <v>700</v>
       </c>
       <c r="J32">
-        <v>2350</v>
+        <v>480</v>
       </c>
       <c r="K32">
         <f t="shared" si="7"/>
-        <v>4150</v>
+        <v>400</v>
       </c>
       <c r="L32" s="8">
         <f t="shared" si="8"/>
-        <v>0.72289156626506024</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.4">
@@ -4893,15 +4915,15 @@
         <v>700</v>
       </c>
       <c r="J33">
-        <v>2400</v>
+        <v>490</v>
       </c>
       <c r="K33">
         <f t="shared" si="7"/>
-        <v>4200</v>
+        <v>410</v>
       </c>
       <c r="L33" s="8">
         <f t="shared" si="8"/>
-        <v>0.7142857142857143</v>
+        <v>0.48780487804878048</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.4">
@@ -4932,15 +4954,15 @@
         <v>700</v>
       </c>
       <c r="J34">
-        <v>2450</v>
+        <v>500</v>
       </c>
       <c r="K34">
         <f t="shared" si="7"/>
-        <v>4250</v>
+        <v>420</v>
       </c>
       <c r="L34" s="8">
         <f t="shared" si="8"/>
-        <v>0.70588235294117652</v>
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.4">
@@ -4971,15 +4993,15 @@
         <v>800</v>
       </c>
       <c r="J35">
-        <v>2500</v>
+        <v>510</v>
       </c>
       <c r="K35">
         <f t="shared" si="7"/>
-        <v>4300</v>
+        <v>430</v>
       </c>
       <c r="L35" s="8">
         <f t="shared" si="8"/>
-        <v>0.69767441860465118</v>
+        <v>0.46511627906976744</v>
       </c>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.4">
@@ -5010,15 +5032,15 @@
         <v>800</v>
       </c>
       <c r="J36">
-        <v>2550</v>
+        <v>520</v>
       </c>
       <c r="K36">
         <f t="shared" si="7"/>
-        <v>4350</v>
+        <v>440</v>
       </c>
       <c r="L36" s="8">
         <f t="shared" si="8"/>
-        <v>0.68965517241379315</v>
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.4">
@@ -5049,15 +5071,15 @@
         <v>800</v>
       </c>
       <c r="J37">
-        <v>2600</v>
+        <v>530</v>
       </c>
       <c r="K37">
         <f t="shared" si="7"/>
-        <v>4400</v>
+        <v>450</v>
       </c>
       <c r="L37" s="8">
         <f t="shared" si="8"/>
-        <v>0.68181818181818177</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.4">
@@ -5088,15 +5110,15 @@
         <v>900</v>
       </c>
       <c r="J38">
-        <v>2650</v>
+        <v>540</v>
       </c>
       <c r="K38">
         <f t="shared" si="7"/>
-        <v>4450</v>
+        <v>460</v>
       </c>
       <c r="L38" s="8">
         <f t="shared" si="8"/>
-        <v>0.6741573033707865</v>
+        <v>0.43478260869565216</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.4">
@@ -5127,15 +5149,15 @@
         <v>900</v>
       </c>
       <c r="J39">
-        <v>2700</v>
+        <v>550</v>
       </c>
       <c r="K39">
         <f t="shared" si="7"/>
-        <v>4500</v>
+        <v>470</v>
       </c>
       <c r="L39" s="8">
         <f t="shared" si="8"/>
-        <v>0.66666666666666663</v>
+        <v>0.42553191489361702</v>
       </c>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.4">
@@ -5166,15 +5188,15 @@
         <v>900</v>
       </c>
       <c r="J40">
-        <v>2750</v>
+        <v>560</v>
       </c>
       <c r="K40">
         <f t="shared" si="7"/>
-        <v>4550</v>
+        <v>480</v>
       </c>
       <c r="L40" s="8">
         <f t="shared" si="8"/>
-        <v>0.65934065934065933</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.4">
@@ -5205,15 +5227,15 @@
         <v>1000</v>
       </c>
       <c r="J41">
-        <v>2800</v>
+        <v>570</v>
       </c>
       <c r="K41">
         <f t="shared" si="7"/>
-        <v>4600</v>
+        <v>490</v>
       </c>
       <c r="L41" s="8">
         <f t="shared" si="8"/>
-        <v>0.65217391304347827</v>
+        <v>0.40816326530612246</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.4">
@@ -5244,15 +5266,15 @@
         <v>1000</v>
       </c>
       <c r="J42">
-        <v>2850</v>
+        <v>580</v>
       </c>
       <c r="K42">
         <f t="shared" si="7"/>
-        <v>4650</v>
+        <v>500</v>
       </c>
       <c r="L42" s="8">
         <f t="shared" si="8"/>
-        <v>0.64516129032258063</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.4">
@@ -5283,15 +5305,15 @@
         <v>1000</v>
       </c>
       <c r="J43">
-        <v>2900</v>
+        <v>590</v>
       </c>
       <c r="K43">
         <f t="shared" si="7"/>
-        <v>4700</v>
+        <v>510</v>
       </c>
       <c r="L43" s="8">
         <f t="shared" si="8"/>
-        <v>0.63829787234042556</v>
+        <v>0.39215686274509803</v>
       </c>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.4">
@@ -5354,15 +5376,15 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <v>3000</v>
+        <v>620</v>
       </c>
       <c r="K45">
         <f t="shared" ref="K45:K54" si="14">$J45-$O$7+$N$7</f>
-        <v>4800</v>
+        <v>540</v>
       </c>
       <c r="L45" s="8">
         <f t="shared" ref="L45:L54" si="15">IF($N$4+$N$7&gt;=$K45,100%,($N$4+$N$7)/$K45)</f>
-        <v>0.625</v>
+        <v>0.37037037037037035</v>
       </c>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.4">
@@ -5393,15 +5415,15 @@
         <v>1500</v>
       </c>
       <c r="J46">
-        <v>3100</v>
+        <v>640</v>
       </c>
       <c r="K46">
         <f t="shared" si="14"/>
-        <v>4900</v>
+        <v>560</v>
       </c>
       <c r="L46" s="8">
         <f t="shared" si="15"/>
-        <v>0.61224489795918369</v>
+        <v>0.35714285714285715</v>
       </c>
     </row>
     <row r="47" spans="3:12" x14ac:dyDescent="0.4">
@@ -5432,15 +5454,15 @@
         <v>1600</v>
       </c>
       <c r="J47">
-        <v>3200</v>
+        <v>660</v>
       </c>
       <c r="K47">
         <f t="shared" si="14"/>
-        <v>5000</v>
+        <v>580</v>
       </c>
       <c r="L47" s="8">
         <f t="shared" si="15"/>
-        <v>0.6</v>
+        <v>0.34482758620689657</v>
       </c>
     </row>
     <row r="48" spans="3:12" x14ac:dyDescent="0.4">
@@ -5471,15 +5493,15 @@
         <v>1700</v>
       </c>
       <c r="J48">
-        <v>3300</v>
+        <v>680</v>
       </c>
       <c r="K48">
         <f t="shared" si="14"/>
-        <v>5100</v>
+        <v>600</v>
       </c>
       <c r="L48" s="8">
         <f t="shared" si="15"/>
-        <v>0.58823529411764708</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="49" spans="3:12" x14ac:dyDescent="0.4">
@@ -5510,15 +5532,15 @@
         <v>1800</v>
       </c>
       <c r="J49">
-        <v>3400</v>
+        <v>700</v>
       </c>
       <c r="K49">
         <f t="shared" si="14"/>
-        <v>5200</v>
+        <v>620</v>
       </c>
       <c r="L49" s="8">
         <f t="shared" si="15"/>
-        <v>0.57692307692307687</v>
+        <v>0.32258064516129031</v>
       </c>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.4">
@@ -5549,15 +5571,15 @@
         <v>1900</v>
       </c>
       <c r="J50">
-        <v>3500</v>
+        <v>720</v>
       </c>
       <c r="K50">
         <f t="shared" si="14"/>
-        <v>5300</v>
+        <v>640</v>
       </c>
       <c r="L50" s="8">
         <f t="shared" si="15"/>
-        <v>0.56603773584905659</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.4">
@@ -5588,15 +5610,15 @@
         <v>2000</v>
       </c>
       <c r="J51">
-        <v>3600</v>
+        <v>740</v>
       </c>
       <c r="K51">
         <f t="shared" si="14"/>
-        <v>5400</v>
+        <v>660</v>
       </c>
       <c r="L51" s="8">
         <f t="shared" si="15"/>
-        <v>0.55555555555555558</v>
+        <v>0.30303030303030304</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.4">
@@ -5627,15 +5649,15 @@
         <v>2100</v>
       </c>
       <c r="J52">
-        <v>3700</v>
+        <v>760</v>
       </c>
       <c r="K52">
         <f t="shared" si="14"/>
-        <v>5500</v>
+        <v>680</v>
       </c>
       <c r="L52" s="8">
         <f t="shared" si="15"/>
-        <v>0.54545454545454541</v>
+        <v>0.29411764705882354</v>
       </c>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.4">
@@ -5666,15 +5688,15 @@
         <v>2200</v>
       </c>
       <c r="J53">
-        <v>3800</v>
+        <v>780</v>
       </c>
       <c r="K53">
         <f t="shared" si="14"/>
-        <v>5600</v>
+        <v>700</v>
       </c>
       <c r="L53" s="8">
         <f t="shared" si="15"/>
-        <v>0.5357142857142857</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.4">
@@ -5705,15 +5727,15 @@
         <v>2300</v>
       </c>
       <c r="J54">
-        <v>3900</v>
+        <v>800</v>
       </c>
       <c r="K54">
         <f t="shared" si="14"/>
-        <v>5700</v>
+        <v>720</v>
       </c>
       <c r="L54" s="8">
         <f t="shared" si="15"/>
-        <v>0.52631578947368418</v>
+        <v>0.27777777777777779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed :: Wrong value
.
</commit_message>
<xml_diff>
--- a/검 강화 게임.xlsx
+++ b/검 강화 게임.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\문서\GitHub\Unity_Weapon_Forge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897D3F40-36EB-42AA-BC8A-EC9ABA929F9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9E3DBA-40CC-467A-BD4A-FC0CABF35239}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8856" xr2:uid="{D3FEDBA6-35E5-45CF-B54A-9F527DCBFA6E}"/>
   </bookViews>
@@ -1348,154 +1348,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>168</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>330</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>598</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>972</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1508</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2256</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3219</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4447</c:v>
+                  <c:v>4150</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5996</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7863</c:v>
+                  <c:v>7350</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10101</c:v>
+                  <c:v>9450</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12766</c:v>
+                  <c:v>11950</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15855</c:v>
+                  <c:v>14850</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19424</c:v>
+                  <c:v>18200</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23523</c:v>
+                  <c:v>22050</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>28152</c:v>
+                  <c:v>26400</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>33364</c:v>
+                  <c:v>31300</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>69846</c:v>
+                  <c:v>65700</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39520</c:v>
+                  <c:v>37000</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>46652</c:v>
+                  <c:v>43700</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>54844</c:v>
+                  <c:v>51400</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>64202</c:v>
+                  <c:v>60200</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>74832</c:v>
+                  <c:v>70200</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>86746</c:v>
+                  <c:v>81400</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>100038</c:v>
+                  <c:v>93900</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>114820</c:v>
+                  <c:v>107800</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>131086</c:v>
+                  <c:v>123100</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>148942</c:v>
+                  <c:v>139900</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>168494</c:v>
+                  <c:v>158300</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>189748</c:v>
+                  <c:v>178300</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>212804</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>237768</c:v>
+                  <c:v>223500</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>264646</c:v>
+                  <c:v>248800</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>293538</c:v>
+                  <c:v>276000</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>324550</c:v>
+                  <c:v>305200</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>357688</c:v>
+                  <c:v>336400</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>637382</c:v>
+                  <c:v>600200</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>394106</c:v>
+                  <c:v>370100</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>433294</c:v>
+                  <c:v>406900</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>475980</c:v>
+                  <c:v>447000</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>522376</c:v>
+                  <c:v>490600</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>572694</c:v>
+                  <c:v>537900</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>627146</c:v>
+                  <c:v>589100</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>686064</c:v>
+                  <c:v>644400</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>749540</c:v>
+                  <c:v>704000</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>817786</c:v>
+                  <c:v>768100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1543,154 +1543,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>230</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>560</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1158</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2130</c:v>
+                  <c:v>1950</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3638</c:v>
+                  <c:v>3350</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5894</c:v>
+                  <c:v>5450</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9113</c:v>
+                  <c:v>8450</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13560</c:v>
+                  <c:v>12600</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19556</c:v>
+                  <c:v>18200</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27419</c:v>
+                  <c:v>25550</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37520</c:v>
+                  <c:v>35000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50286</c:v>
+                  <c:v>46950</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>66141</c:v>
+                  <c:v>61800</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>85565</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>109088</c:v>
+                  <c:v>102050</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>137240</c:v>
+                  <c:v>128450</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>170604</c:v>
+                  <c:v>159750</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>240450</c:v>
+                  <c:v>225450</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>279970</c:v>
+                  <c:v>262450</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>326622</c:v>
+                  <c:v>306150</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>381466</c:v>
+                  <c:v>357550</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>445668</c:v>
+                  <c:v>417750</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>520500</c:v>
+                  <c:v>487950</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>607246</c:v>
+                  <c:v>569350</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>707284</c:v>
+                  <c:v>663250</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>822104</c:v>
+                  <c:v>771050</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>953190</c:v>
+                  <c:v>894150</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1102132</c:v>
+                  <c:v>1034050</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1270626</c:v>
+                  <c:v>1192350</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1460374</c:v>
+                  <c:v>1370650</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1673178</c:v>
+                  <c:v>1570650</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1910946</c:v>
+                  <c:v>1794150</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2175592</c:v>
+                  <c:v>2042950</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2469130</c:v>
+                  <c:v>2318950</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2793680</c:v>
+                  <c:v>2624150</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3151368</c:v>
+                  <c:v>2960550</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3788750</c:v>
+                  <c:v>3560750</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4182856</c:v>
+                  <c:v>3930850</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4616150</c:v>
+                  <c:v>4337750</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5092130</c:v>
+                  <c:v>4784750</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5614506</c:v>
+                  <c:v>5275350</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6187200</c:v>
+                  <c:v>5813250</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6814346</c:v>
+                  <c:v>6402350</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>7500410</c:v>
+                  <c:v>7046750</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>8249950</c:v>
+                  <c:v>7750750</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>9067736</c:v>
+                  <c:v>8518850</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2004,154 +2004,154 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.95238095238095233</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.90909090909090906</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.86956521739130432</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97826086956521741</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.95238095238095233</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.92783505154639179</c:v>
+                  <c:v>0.76923076923076927</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.90452261306532666</c:v>
+                  <c:v>0.7407407407407407</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.88235294117647056</c:v>
+                  <c:v>0.7142857142857143</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.86124401913875603</c:v>
+                  <c:v>0.68965517241379315</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.84112149532710279</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.82191780821917804</c:v>
+                  <c:v>0.64516129032258063</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.8035714285714286</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.78602620087336239</c:v>
+                  <c:v>0.60606060606060608</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.76923076923076927</c:v>
+                  <c:v>0.58823529411764708</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.7531380753138075</c:v>
+                  <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.73770491803278693</c:v>
+                  <c:v>0.55555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.72289156626506024</c:v>
+                  <c:v>0.54054054054054057</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.70866141732283461</c:v>
+                  <c:v>0.52631578947368418</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.69498069498069504</c:v>
+                  <c:v>0.51282051282051277</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.66914498141263945</c:v>
+                  <c:v>0.48780487804878048</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.65693430656934304</c:v>
+                  <c:v>0.47619047619047616</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.64516129032258063</c:v>
+                  <c:v>0.46511627906976744</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.63380281690140849</c:v>
+                  <c:v>0.45454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.62283737024221453</c:v>
+                  <c:v>0.44444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.61224489795918369</c:v>
+                  <c:v>0.43478260869565216</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.60200668896321075</c:v>
+                  <c:v>0.42553191489361702</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.59210526315789469</c:v>
+                  <c:v>0.41666666666666669</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.58252427184466016</c:v>
+                  <c:v>0.40816326530612246</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.57324840764331209</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.56426332288401249</c:v>
+                  <c:v>0.39215686274509803</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.55555555555555558</c:v>
+                  <c:v>0.38461538461538464</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.54711246200607899</c:v>
+                  <c:v>0.37735849056603776</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.53892215568862278</c:v>
+                  <c:v>0.37037037037037035</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.53097345132743368</c:v>
+                  <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.52325581395348841</c:v>
+                  <c:v>0.35714285714285715</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.51575931232091687</c:v>
+                  <c:v>0.35087719298245612</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.50847457627118642</c:v>
+                  <c:v>0.34482758620689657</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.50139275766016711</c:v>
+                  <c:v>0.33898305084745761</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.48128342245989303</c:v>
+                  <c:v>0.32258064516129031</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.46875</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.45685279187817257</c:v>
+                  <c:v>0.30303030303030304</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.44554455445544555</c:v>
+                  <c:v>0.29411764705882354</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.43478260869565216</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.42452830188679247</c:v>
+                  <c:v>0.27777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.41474654377880182</c:v>
+                  <c:v>0.27027027027027029</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.40540540540540543</c:v>
+                  <c:v>0.26315789473684209</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.3964757709251101</c:v>
+                  <c:v>0.25641025641025639</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.38793103448275862</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4843,8 +4843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62FF258-7648-4ED0-AA06-DFEB56F203C0}">
   <dimension ref="C2:AO54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="71" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="P2" zoomScale="71" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AS7" sqref="AS7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4979,7 +4979,7 @@
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K23" si="0">$J4-$S$7+$R$7</f>
-        <v>328</v>
+        <v>200</v>
       </c>
       <c r="L4" s="14">
         <f t="shared" ref="L4:L23" si="1">IF($R$4+$R$7&gt;=$K4,100%,($R$4+$R$7)/$K4)</f>
@@ -5050,19 +5050,19 @@
       </c>
       <c r="E5" s="1">
         <f>50*(100+$U$7)/100</f>
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5:F23" si="3">E5-D4-E4</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ref="G5:G23" si="4">F5+G4</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H23" si="5">F5-F4</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -5072,11 +5072,11 @@
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>210</v>
       </c>
       <c r="L5" s="14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.95238095238095233</v>
       </c>
       <c r="M5">
         <v>0.4</v>
@@ -5108,18 +5108,18 @@
         <v>32</v>
       </c>
       <c r="AD5" s="1">
-        <f>$AC4+$AD4</f>
+        <f t="shared" ref="AD5:AD24" si="11">$AC4+$AD4</f>
         <v>32</v>
       </c>
       <c r="AE5" s="1">
         <v>2</v>
       </c>
       <c r="AF5" s="1">
-        <f>$AF4+$AE4</f>
+        <f t="shared" ref="AF5:AF24" si="12">$AF4+$AE4</f>
         <v>1</v>
       </c>
       <c r="AL5" s="2">
-        <f t="shared" ref="AL5:AL24" si="11">AL4+1</f>
+        <f t="shared" ref="AL5:AL24" si="13">AL4+1</f>
         <v>1</v>
       </c>
       <c r="AM5" s="1">
@@ -5129,7 +5129,7 @@
         <v>16</v>
       </c>
       <c r="AO5" s="1">
-        <f t="shared" ref="AO5:AO24" si="12">$AN5+$AO4</f>
+        <f t="shared" ref="AO5:AO24" si="14">$AN5+$AO4</f>
         <v>16</v>
       </c>
     </row>
@@ -5143,34 +5143,34 @@
       </c>
       <c r="E6" s="1">
         <f>200*(100+$U$7)/100</f>
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F6" s="1">
         <f>E6-D5-E5</f>
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="5"/>
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I6:I23" si="13">H6-H5-I5</f>
-        <v>53</v>
+        <f t="shared" ref="I6:I23" si="15">H6-H5-I5</f>
+        <v>50</v>
       </c>
       <c r="J6">
         <v>220</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>348</v>
+        <v>220</v>
       </c>
       <c r="L6" s="14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="M6">
         <v>0.6</v>
@@ -5211,18 +5211,18 @@
         <v>32</v>
       </c>
       <c r="AD6" s="1">
-        <f>$AC5+$AD5</f>
+        <f t="shared" si="11"/>
         <v>64</v>
       </c>
       <c r="AE6" s="1">
         <v>3</v>
       </c>
       <c r="AF6" s="1">
-        <f>$AF5+$AE5</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="AL6" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="AM6" s="1">
@@ -5232,7 +5232,7 @@
         <v>16</v>
       </c>
       <c r="AO6" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>32</v>
       </c>
     </row>
@@ -5246,22 +5246,22 @@
       </c>
       <c r="E7" s="1">
         <f>500*(100+$U$7)/100</f>
-        <v>530</v>
+        <v>500</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="3"/>
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="4"/>
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="5"/>
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="J7">
@@ -5269,11 +5269,11 @@
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>358</v>
+        <v>230</v>
       </c>
       <c r="L7" s="14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.86956521739130432</v>
       </c>
       <c r="M7">
         <v>0.8</v>
@@ -5292,15 +5292,15 @@
       </c>
       <c r="R7">
         <f>INDEX(Z4:AF24,MATCH($R$11, $Z4:$Z24), 5)</f>
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <f>INDEX(AL4:AO24,MATCH($R$14, $AL4:$AL24), 4)</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="U7">
         <f>INDEX(Z4:AF24,MATCH($S$11, $Z4:$Z24), 7)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="2">
         <f t="shared" si="9"/>
@@ -5317,18 +5317,18 @@
         <v>32</v>
       </c>
       <c r="AD7" s="1">
-        <f>$AC6+$AD6</f>
+        <f t="shared" si="11"/>
         <v>96</v>
       </c>
       <c r="AE7" s="1">
         <v>4</v>
       </c>
       <c r="AF7" s="1">
-        <f>$AF6+$AE6</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="AL7" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="AM7" s="1">
@@ -5338,7 +5338,7 @@
         <v>16</v>
       </c>
       <c r="AO7" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>48</v>
       </c>
     </row>
@@ -5352,34 +5352,34 @@
       </c>
       <c r="E8" s="1">
         <f>1000*(100+$U$7)/100</f>
-        <v>1060</v>
+        <v>1000</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="3"/>
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="4"/>
-        <v>560</v>
+        <v>500</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="5"/>
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="13"/>
-        <v>53</v>
+        <f t="shared" si="15"/>
+        <v>50</v>
       </c>
       <c r="J8">
         <v>240</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="L8" s="14">
         <f t="shared" si="1"/>
-        <v>0.97826086956521741</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -5411,18 +5411,18 @@
         <v>32</v>
       </c>
       <c r="AD8" s="1">
-        <f>$AC7+$AD7</f>
+        <f t="shared" si="11"/>
         <v>128</v>
       </c>
       <c r="AE8" s="1">
         <v>5</v>
       </c>
       <c r="AF8" s="1">
-        <f>$AF7+$AE7</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="AL8" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="AM8" s="1">
@@ -5432,7 +5432,7 @@
         <v>16</v>
       </c>
       <c r="AO8" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
     </row>
@@ -5446,34 +5446,34 @@
       </c>
       <c r="E9" s="1">
         <f>1800*(100+$U$7)/100</f>
-        <v>1908</v>
+        <v>1800</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="3"/>
-        <v>598</v>
+        <v>550</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="4"/>
-        <v>1158</v>
+        <v>1050</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="5"/>
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="13"/>
-        <v>53</v>
+        <f t="shared" si="15"/>
+        <v>50</v>
       </c>
       <c r="J9">
         <v>250</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>378</v>
+        <v>250</v>
       </c>
       <c r="L9" s="14">
         <f t="shared" si="1"/>
-        <v>0.95238095238095233</v>
+        <v>0.8</v>
       </c>
       <c r="M9">
         <v>1.2</v>
@@ -5505,18 +5505,18 @@
         <v>32</v>
       </c>
       <c r="AD9" s="1">
-        <f>$AC8+$AD8</f>
+        <f t="shared" si="11"/>
         <v>160</v>
       </c>
       <c r="AE9" s="1">
         <v>6</v>
       </c>
       <c r="AF9" s="1">
-        <f>$AF8+$AE8</f>
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
       <c r="AL9" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="AM9" s="1">
@@ -5526,7 +5526,7 @@
         <v>16</v>
       </c>
       <c r="AO9" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>80</v>
       </c>
     </row>
@@ -5540,34 +5540,34 @@
       </c>
       <c r="E10" s="1">
         <f>3000*(100+$U$7)/100</f>
-        <v>3180</v>
+        <v>3000</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="3"/>
-        <v>972</v>
+        <v>900</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="4"/>
-        <v>2130</v>
+        <v>1950</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="5"/>
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="13"/>
-        <v>53</v>
+        <f t="shared" si="15"/>
+        <v>50</v>
       </c>
       <c r="J10">
         <v>260</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>388</v>
+        <v>260</v>
       </c>
       <c r="L10" s="14">
         <f t="shared" si="1"/>
-        <v>0.92783505154639179</v>
+        <v>0.76923076923076927</v>
       </c>
       <c r="M10">
         <v>1.4</v>
@@ -5605,18 +5605,18 @@
         <v>32</v>
       </c>
       <c r="AD10" s="1">
-        <f>$AC9+$AD9</f>
+        <f t="shared" si="11"/>
         <v>192</v>
       </c>
       <c r="AE10" s="1">
         <v>7</v>
       </c>
       <c r="AF10" s="1">
-        <f>$AF9+$AE9</f>
+        <f t="shared" si="12"/>
         <v>21</v>
       </c>
       <c r="AL10" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="AM10" s="1">
@@ -5626,7 +5626,7 @@
         <v>16</v>
       </c>
       <c r="AO10" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>96</v>
       </c>
     </row>
@@ -5640,34 +5640,34 @@
       </c>
       <c r="E11" s="1">
         <f>4800*(100+$U$7)/100</f>
-        <v>5088</v>
+        <v>4800</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="3"/>
-        <v>1508</v>
+        <v>1400</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="4"/>
-        <v>3638</v>
+        <v>3350</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="5"/>
-        <v>536</v>
+        <v>500</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="13"/>
-        <v>109</v>
+        <f t="shared" si="15"/>
+        <v>100</v>
       </c>
       <c r="J11">
         <v>270</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>398</v>
+        <v>270</v>
       </c>
       <c r="L11" s="14">
         <f t="shared" si="1"/>
-        <v>0.90452261306532666</v>
+        <v>0.7407407407407407</v>
       </c>
       <c r="M11">
         <v>1.6</v>
@@ -5685,10 +5685,10 @@
         <v>2.6000000000000005</v>
       </c>
       <c r="R11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="2">
         <f t="shared" si="9"/>
@@ -5705,18 +5705,18 @@
         <v>32</v>
       </c>
       <c r="AD11" s="1">
-        <f>$AC10+$AD10</f>
+        <f t="shared" si="11"/>
         <v>224</v>
       </c>
       <c r="AE11" s="1">
         <v>8</v>
       </c>
       <c r="AF11" s="1">
-        <f>$AF10+$AE10</f>
+        <f t="shared" si="12"/>
         <v>28</v>
       </c>
       <c r="AL11" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="AM11" s="1">
@@ -5726,7 +5726,7 @@
         <v>16</v>
       </c>
       <c r="AO11" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>112</v>
       </c>
     </row>
@@ -5740,34 +5740,34 @@
       </c>
       <c r="E12" s="1">
         <f>7400*(100+$U$7)/100</f>
-        <v>7844</v>
+        <v>7400</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="3"/>
-        <v>2256</v>
+        <v>2100</v>
       </c>
       <c r="G12" s="1">
         <f>F12+G11</f>
-        <v>5894</v>
+        <v>5450</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="5"/>
-        <v>748</v>
+        <v>700</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="13"/>
-        <v>103</v>
+        <f t="shared" si="15"/>
+        <v>100</v>
       </c>
       <c r="J12">
         <v>280</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>408</v>
+        <v>280</v>
       </c>
       <c r="L12" s="14">
         <f t="shared" si="1"/>
-        <v>0.88235294117647056</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="M12">
         <v>1.8</v>
@@ -5799,18 +5799,18 @@
         <v>32</v>
       </c>
       <c r="AD12" s="1">
-        <f>$AC11+$AD11</f>
+        <f t="shared" si="11"/>
         <v>256</v>
       </c>
       <c r="AE12" s="1">
         <v>9</v>
       </c>
       <c r="AF12" s="1">
-        <f>$AF11+$AE11</f>
+        <f t="shared" si="12"/>
         <v>36</v>
       </c>
       <c r="AL12" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="AM12" s="1">
@@ -5820,7 +5820,7 @@
         <v>16</v>
       </c>
       <c r="AO12" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>128</v>
       </c>
     </row>
@@ -5834,34 +5834,34 @@
       </c>
       <c r="E13" s="1">
         <f>11050*(100+$U$7)/100</f>
-        <v>11713</v>
+        <v>11050</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="3"/>
-        <v>3219</v>
+        <v>3000</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="4"/>
-        <v>9113</v>
+        <v>8450</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="5"/>
-        <v>963</v>
+        <v>900</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="13"/>
-        <v>112</v>
+        <f t="shared" si="15"/>
+        <v>100</v>
       </c>
       <c r="J13">
         <v>290</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>418</v>
+        <v>290</v>
       </c>
       <c r="L13" s="14">
         <f t="shared" si="1"/>
-        <v>0.86124401913875603</v>
+        <v>0.68965517241379315</v>
       </c>
       <c r="M13">
         <v>2</v>
@@ -5896,18 +5896,18 @@
         <v>64</v>
       </c>
       <c r="AD13" s="1">
-        <f>$AC12+$AD12</f>
+        <f t="shared" si="11"/>
         <v>288</v>
       </c>
       <c r="AE13" s="1">
         <v>10</v>
       </c>
       <c r="AF13" s="1">
-        <f>$AF12+$AE12</f>
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
       <c r="AL13" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="AM13" s="1">
@@ -5917,7 +5917,7 @@
         <v>16</v>
       </c>
       <c r="AO13" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>144</v>
       </c>
     </row>
@@ -5931,34 +5931,34 @@
       </c>
       <c r="E14" s="1">
         <f>16000*(100+$U$7)/100</f>
-        <v>16960</v>
+        <v>16000</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="3"/>
-        <v>4447</v>
+        <v>4150</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="4"/>
-        <v>13560</v>
+        <v>12600</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="5"/>
-        <v>1228</v>
+        <v>1150</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="13"/>
-        <v>153</v>
+        <f t="shared" si="15"/>
+        <v>150</v>
       </c>
       <c r="J14">
         <v>300</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>428</v>
+        <v>300</v>
       </c>
       <c r="L14" s="14">
         <f t="shared" si="1"/>
-        <v>0.84112149532710279</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M14" s="10">
         <v>2.5</v>
@@ -5976,7 +5976,7 @@
         <v>3.8000000000000007</v>
       </c>
       <c r="R14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="2">
         <f t="shared" si="9"/>
@@ -5993,19 +5993,19 @@
         <v>32</v>
       </c>
       <c r="AD14" s="1">
-        <f>$AC13+$AD13</f>
+        <f t="shared" si="11"/>
         <v>352</v>
       </c>
       <c r="AE14" s="1">
         <v>11</v>
       </c>
       <c r="AF14" s="1">
-        <f>$AF13+$AE13</f>
+        <f t="shared" si="12"/>
         <v>55</v>
       </c>
       <c r="AJ14" s="11"/>
       <c r="AL14" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="AM14" s="1">
@@ -6015,7 +6015,7 @@
         <v>16</v>
       </c>
       <c r="AO14" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>160</v>
       </c>
     </row>
@@ -6029,34 +6029,34 @@
       </c>
       <c r="E15" s="1">
         <f>22600*(100+$U$7)/100</f>
-        <v>23956</v>
+        <v>22600</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="3"/>
-        <v>5996</v>
+        <v>5600</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="4"/>
-        <v>19556</v>
+        <v>18200</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="5"/>
-        <v>1549</v>
+        <v>1450</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="13"/>
-        <v>168</v>
+        <f t="shared" si="15"/>
+        <v>150</v>
       </c>
       <c r="J15">
         <v>310</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>438</v>
+        <v>310</v>
       </c>
       <c r="L15" s="14">
         <f t="shared" si="1"/>
-        <v>0.82191780821917804</v>
+        <v>0.64516129032258063</v>
       </c>
       <c r="M15">
         <v>3</v>
@@ -6088,18 +6088,18 @@
         <v>32</v>
       </c>
       <c r="AD15" s="1">
-        <f>$AC14+$AD14</f>
+        <f t="shared" si="11"/>
         <v>384</v>
       </c>
       <c r="AE15" s="1">
         <v>12</v>
       </c>
       <c r="AF15" s="1">
-        <f>$AF14+$AE14</f>
+        <f t="shared" si="12"/>
         <v>66</v>
       </c>
       <c r="AL15" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="AM15" s="1">
@@ -6109,7 +6109,7 @@
         <v>16</v>
       </c>
       <c r="AO15" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>176</v>
       </c>
     </row>
@@ -6123,22 +6123,22 @@
       </c>
       <c r="E16" s="1">
         <f>31150*(100+$U$7)/100</f>
-        <v>33019</v>
+        <v>31150</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="3"/>
-        <v>7863</v>
+        <v>7350</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="4"/>
-        <v>27419</v>
+        <v>25550</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="5"/>
-        <v>1867</v>
+        <v>1750</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>150</v>
       </c>
       <c r="J16">
@@ -6146,11 +6146,11 @@
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>448</v>
+        <v>320</v>
       </c>
       <c r="L16" s="14">
         <f t="shared" si="1"/>
-        <v>0.8035714285714286</v>
+        <v>0.625</v>
       </c>
       <c r="M16">
         <v>3.5</v>
@@ -6182,18 +6182,18 @@
         <v>32</v>
       </c>
       <c r="AD16" s="1">
-        <f>$AC15+$AD15</f>
+        <f t="shared" si="11"/>
         <v>416</v>
       </c>
       <c r="AE16" s="1">
         <v>13</v>
       </c>
       <c r="AF16" s="1">
-        <f>$AF15+$AE15</f>
+        <f t="shared" si="12"/>
         <v>78</v>
       </c>
       <c r="AL16" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
       <c r="AM16" s="1">
@@ -6203,7 +6203,7 @@
         <v>16</v>
       </c>
       <c r="AO16" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>192</v>
       </c>
     </row>
@@ -6217,34 +6217,34 @@
       </c>
       <c r="E17" s="1">
         <f>42000*(100+$U$7)/100</f>
-        <v>44520</v>
+        <v>42000</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="3"/>
-        <v>10101</v>
+        <v>9450</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="4"/>
-        <v>37520</v>
+        <v>35000</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="5"/>
-        <v>2238</v>
+        <v>2100</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="13"/>
-        <v>221</v>
+        <f t="shared" si="15"/>
+        <v>200</v>
       </c>
       <c r="J17">
         <v>330</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>458</v>
+        <v>330</v>
       </c>
       <c r="L17" s="14">
         <f t="shared" si="1"/>
-        <v>0.78602620087336239</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="M17">
         <v>4</v>
@@ -6276,18 +6276,18 @@
         <v>32</v>
       </c>
       <c r="AD17" s="1">
-        <f>$AC16+$AD16</f>
+        <f t="shared" si="11"/>
         <v>448</v>
       </c>
       <c r="AE17" s="1">
         <v>14</v>
       </c>
       <c r="AF17" s="1">
-        <f>$AF16+$AE16</f>
+        <f t="shared" si="12"/>
         <v>91</v>
       </c>
       <c r="AL17" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>13</v>
       </c>
       <c r="AM17" s="1">
@@ -6297,7 +6297,7 @@
         <v>16</v>
       </c>
       <c r="AO17" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>208</v>
       </c>
     </row>
@@ -6311,34 +6311,34 @@
       </c>
       <c r="E18" s="1">
         <f>55600*(100+$U$7)/100</f>
-        <v>58936</v>
+        <v>55600</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="3"/>
-        <v>12766</v>
+        <v>11950</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="4"/>
-        <v>50286</v>
+        <v>46950</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="5"/>
-        <v>2665</v>
+        <v>2500</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="13"/>
-        <v>206</v>
+        <f t="shared" si="15"/>
+        <v>200</v>
       </c>
       <c r="J18">
         <v>340</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>468</v>
+        <v>340</v>
       </c>
       <c r="L18" s="14">
         <f t="shared" si="1"/>
-        <v>0.76923076923076927</v>
+        <v>0.58823529411764708</v>
       </c>
       <c r="M18">
         <v>4.5</v>
@@ -6370,18 +6370,18 @@
         <v>32</v>
       </c>
       <c r="AD18" s="1">
-        <f>$AC17+$AD17</f>
+        <f t="shared" si="11"/>
         <v>480</v>
       </c>
       <c r="AE18" s="1">
         <v>15</v>
       </c>
       <c r="AF18" s="1">
-        <f>$AF17+$AE17</f>
+        <f t="shared" si="12"/>
         <v>105</v>
       </c>
       <c r="AL18" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="AM18" s="1">
@@ -6391,7 +6391,7 @@
         <v>16</v>
       </c>
       <c r="AO18" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>224</v>
       </c>
     </row>
@@ -6405,34 +6405,34 @@
       </c>
       <c r="E19" s="1">
         <f>72350*(100+$U$7)/100</f>
-        <v>76691</v>
+        <v>72350</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="3"/>
-        <v>15855</v>
+        <v>14850</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="4"/>
-        <v>66141</v>
+        <v>61800</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="5"/>
-        <v>3089</v>
+        <v>2900</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="13"/>
-        <v>218</v>
+        <f t="shared" si="15"/>
+        <v>200</v>
       </c>
       <c r="J19">
         <v>350</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>478</v>
+        <v>350</v>
       </c>
       <c r="L19" s="14">
         <f t="shared" si="1"/>
-        <v>0.7531380753138075</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="M19">
         <v>5</v>
@@ -6464,18 +6464,18 @@
         <v>32</v>
       </c>
       <c r="AD19" s="1">
-        <f>$AC18+$AD18</f>
+        <f t="shared" si="11"/>
         <v>512</v>
       </c>
       <c r="AE19" s="1">
         <v>16</v>
       </c>
       <c r="AF19" s="1">
-        <f>$AF18+$AE18</f>
+        <f t="shared" si="12"/>
         <v>120</v>
       </c>
       <c r="AL19" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="AM19" s="1">
@@ -6485,7 +6485,7 @@
         <v>16</v>
       </c>
       <c r="AO19" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>240</v>
       </c>
     </row>
@@ -6499,34 +6499,34 @@
       </c>
       <c r="E20" s="1">
         <f>92750*(100+$U$7)/100</f>
-        <v>98315</v>
+        <v>92750</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="3"/>
-        <v>19424</v>
+        <v>18200</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="4"/>
-        <v>85565</v>
+        <v>80000</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="5"/>
-        <v>3569</v>
+        <v>3350</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="13"/>
-        <v>262</v>
+        <f t="shared" si="15"/>
+        <v>250</v>
       </c>
       <c r="J20">
         <v>360</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>488</v>
+        <v>360</v>
       </c>
       <c r="L20" s="14">
         <f t="shared" si="1"/>
-        <v>0.73770491803278693</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="M20">
         <v>5.5</v>
@@ -6558,18 +6558,18 @@
         <v>32</v>
       </c>
       <c r="AD20" s="1">
-        <f>$AC19+$AD19</f>
+        <f t="shared" si="11"/>
         <v>544</v>
       </c>
       <c r="AE20" s="1">
         <v>17</v>
       </c>
       <c r="AF20" s="1">
-        <f>$AF19+$AE19</f>
+        <f t="shared" si="12"/>
         <v>136</v>
       </c>
       <c r="AL20" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="AM20" s="1">
@@ -6579,7 +6579,7 @@
         <v>16</v>
       </c>
       <c r="AO20" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>256</v>
       </c>
     </row>
@@ -6593,34 +6593,34 @@
       </c>
       <c r="E21" s="1">
         <f>117300*(100+$U$7)/100</f>
-        <v>124338</v>
+        <v>117300</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="3"/>
-        <v>23523</v>
+        <v>22050</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="4"/>
-        <v>109088</v>
+        <v>102050</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="5"/>
-        <v>4099</v>
+        <v>3850</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="13"/>
-        <v>268</v>
+        <f t="shared" si="15"/>
+        <v>250</v>
       </c>
       <c r="J21">
         <v>370</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>498</v>
+        <v>370</v>
       </c>
       <c r="L21" s="14">
         <f t="shared" si="1"/>
-        <v>0.72289156626506024</v>
+        <v>0.54054054054054057</v>
       </c>
       <c r="M21">
         <v>6</v>
@@ -6652,18 +6652,18 @@
         <v>32</v>
       </c>
       <c r="AD21" s="1">
-        <f>$AC20+$AD20</f>
+        <f t="shared" si="11"/>
         <v>576</v>
       </c>
       <c r="AE21" s="1">
         <v>18</v>
       </c>
       <c r="AF21" s="1">
-        <f>$AF20+$AE20</f>
+        <f t="shared" si="12"/>
         <v>153</v>
       </c>
       <c r="AL21" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
       <c r="AM21" s="1">
@@ -6673,7 +6673,7 @@
         <v>16</v>
       </c>
       <c r="AO21" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>272</v>
       </c>
     </row>
@@ -6687,34 +6687,34 @@
       </c>
       <c r="E22" s="1">
         <f>146500*(100+$U$7)/100</f>
-        <v>155290</v>
+        <v>146500</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="3"/>
-        <v>28152</v>
+        <v>26400</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="4"/>
-        <v>137240</v>
+        <v>128450</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="5"/>
-        <v>4629</v>
+        <v>4350</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="13"/>
-        <v>262</v>
+        <f t="shared" si="15"/>
+        <v>250</v>
       </c>
       <c r="J22">
         <v>380</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>508</v>
+        <v>380</v>
       </c>
       <c r="L22" s="14">
         <f t="shared" si="1"/>
-        <v>0.70866141732283461</v>
+        <v>0.52631578947368418</v>
       </c>
       <c r="M22">
         <v>6.5</v>
@@ -6746,18 +6746,18 @@
         <v>32</v>
       </c>
       <c r="AD22" s="1">
-        <f>$AC21+$AD21</f>
+        <f t="shared" si="11"/>
         <v>608</v>
       </c>
       <c r="AE22" s="1">
         <v>19</v>
       </c>
       <c r="AF22" s="1">
-        <f>$AF21+$AE21</f>
+        <f t="shared" si="12"/>
         <v>171</v>
       </c>
       <c r="AL22" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>18</v>
       </c>
       <c r="AM22" s="1">
@@ -6767,7 +6767,7 @@
         <v>16</v>
       </c>
       <c r="AO22" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>288</v>
       </c>
     </row>
@@ -6781,34 +6781,34 @@
       </c>
       <c r="E23" s="1">
         <f>180900*(100+$U$7)/100</f>
-        <v>191754</v>
+        <v>180900</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="3"/>
-        <v>33364</v>
+        <v>31300</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="4"/>
-        <v>170604</v>
+        <v>159750</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="5"/>
-        <v>5212</v>
+        <v>4900</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="13"/>
-        <v>321</v>
+        <f t="shared" si="15"/>
+        <v>300</v>
       </c>
       <c r="J23">
         <v>390</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>518</v>
+        <v>390</v>
       </c>
       <c r="L23" s="14">
         <f t="shared" si="1"/>
-        <v>0.69498069498069504</v>
+        <v>0.51282051282051277</v>
       </c>
       <c r="M23">
         <v>7</v>
@@ -6840,18 +6840,18 @@
         <v>64</v>
       </c>
       <c r="AD23" s="1">
-        <f>$AC22+$AD22</f>
+        <f t="shared" si="11"/>
         <v>640</v>
       </c>
       <c r="AE23" s="1">
         <v>20</v>
       </c>
       <c r="AF23" s="1">
-        <f>$AF22+$AE22</f>
+        <f t="shared" si="12"/>
         <v>190</v>
       </c>
       <c r="AL23" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="AM23" s="1">
@@ -6861,7 +6861,7 @@
         <v>16</v>
       </c>
       <c r="AO23" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>304</v>
       </c>
     </row>
@@ -6923,19 +6923,19 @@
         <v>32</v>
       </c>
       <c r="AD24" s="1">
-        <f>$AC23+$AD23</f>
+        <f t="shared" si="11"/>
         <v>704</v>
       </c>
       <c r="AE24" s="1">
         <v>21</v>
       </c>
       <c r="AF24" s="1">
-        <f>$AF23+$AE23</f>
+        <f t="shared" si="12"/>
         <v>210</v>
       </c>
       <c r="AJ24" s="11"/>
       <c r="AL24" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="AM24" s="12">
@@ -6945,7 +6945,7 @@
         <v>16</v>
       </c>
       <c r="AO24" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>320</v>
       </c>
     </row>
@@ -6959,19 +6959,19 @@
       </c>
       <c r="E25" s="1">
         <f>250000*(100+$U$7)/100</f>
-        <v>265000</v>
+        <v>250000</v>
       </c>
       <c r="F25" s="1">
         <f>E25-D23-E23</f>
-        <v>69846</v>
+        <v>65700</v>
       </c>
       <c r="G25" s="1">
         <f>F25+G23</f>
-        <v>240450</v>
+        <v>225450</v>
       </c>
       <c r="H25" s="1">
         <f>F25-F23</f>
-        <v>36482</v>
+        <v>34400</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -6980,12 +6980,12 @@
         <v>410</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:K43" si="14">$J25-$S$7+$R$7</f>
-        <v>538</v>
+        <f t="shared" ref="K25:K43" si="16">$J25-$S$7+$R$7</f>
+        <v>410</v>
       </c>
       <c r="L25" s="14">
-        <f t="shared" ref="L25:L43" si="15">IF($R$4+$R$7&gt;=$K25,100%,($R$4+$R$7)/$K25)</f>
-        <v>0.66914498141263945</v>
+        <f t="shared" ref="L25:L43" si="17">IF($R$4+$R$7&gt;=$K25,100%,($R$4+$R$7)/$K25)</f>
+        <v>0.48780487804878048</v>
       </c>
       <c r="M25">
         <v>11</v>
@@ -7013,34 +7013,34 @@
       </c>
       <c r="E26" s="1">
         <f>292000*(100+$U$7)/100</f>
-        <v>309520</v>
+        <v>292000</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" ref="F26:F43" si="16">E26-D25-E25</f>
-        <v>39520</v>
+        <f t="shared" ref="F26:F43" si="18">E26-D25-E25</f>
+        <v>37000</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" ref="G26:G43" si="17">F26+G25</f>
-        <v>279970</v>
+        <f t="shared" ref="G26:G43" si="19">F26+G25</f>
+        <v>262450</v>
       </c>
       <c r="H26" s="1">
         <f>F26-F23</f>
-        <v>6156</v>
+        <v>5700</v>
       </c>
       <c r="I26" s="1">
         <f>H26-H23-I23</f>
-        <v>623</v>
+        <v>500</v>
       </c>
       <c r="J26">
         <v>420</v>
       </c>
       <c r="K26">
-        <f t="shared" si="14"/>
-        <v>548</v>
+        <f t="shared" si="16"/>
+        <v>420</v>
       </c>
       <c r="L26" s="14">
-        <f t="shared" si="15"/>
-        <v>0.65693430656934304</v>
+        <f t="shared" si="17"/>
+        <v>0.47619047619047616</v>
       </c>
       <c r="M26">
         <v>12</v>
@@ -7068,34 +7068,34 @@
       </c>
       <c r="E27" s="1">
         <f>341200*(100+$U$7)/100</f>
-        <v>361672</v>
+        <v>341200</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="16"/>
-        <v>46652</v>
+        <f t="shared" si="18"/>
+        <v>43700</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="17"/>
-        <v>326622</v>
+        <f t="shared" si="19"/>
+        <v>306150</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" ref="H27:H43" si="18">F27-F26</f>
-        <v>7132</v>
+        <f t="shared" ref="H27:H43" si="20">F27-F26</f>
+        <v>6700</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" ref="I27:I43" si="19">H27-H26-I26</f>
-        <v>353</v>
+        <f t="shared" ref="I27:I43" si="21">H27-H26-I26</f>
+        <v>500</v>
       </c>
       <c r="J27">
         <v>430</v>
       </c>
       <c r="K27">
-        <f t="shared" si="14"/>
-        <v>558</v>
+        <f t="shared" si="16"/>
+        <v>430</v>
       </c>
       <c r="L27" s="14">
-        <f t="shared" si="15"/>
-        <v>0.64516129032258063</v>
+        <f t="shared" si="17"/>
+        <v>0.46511627906976744</v>
       </c>
       <c r="M27">
         <v>13</v>
@@ -7123,34 +7123,34 @@
       </c>
       <c r="E28" s="1">
         <f>398600*(100+$U$7)/100</f>
-        <v>422516</v>
+        <v>398600</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="16"/>
-        <v>54844</v>
+        <f t="shared" si="18"/>
+        <v>51400</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="17"/>
-        <v>381466</v>
+        <f t="shared" si="19"/>
+        <v>357550</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="18"/>
-        <v>8192</v>
+        <f t="shared" si="20"/>
+        <v>7700</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="19"/>
-        <v>707</v>
+        <f t="shared" si="21"/>
+        <v>500</v>
       </c>
       <c r="J28">
         <v>440</v>
       </c>
       <c r="K28">
-        <f t="shared" si="14"/>
-        <v>568</v>
+        <f t="shared" si="16"/>
+        <v>440</v>
       </c>
       <c r="L28" s="14">
-        <f t="shared" si="15"/>
-        <v>0.63380281690140849</v>
+        <f t="shared" si="17"/>
+        <v>0.45454545454545453</v>
       </c>
       <c r="M28">
         <v>14</v>
@@ -7178,34 +7178,34 @@
       </c>
       <c r="E29" s="1">
         <f>465300*(100+$U$7)/100</f>
-        <v>493218</v>
+        <v>465300</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="16"/>
-        <v>64202</v>
+        <f t="shared" si="18"/>
+        <v>60200</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="17"/>
-        <v>445668</v>
+        <f t="shared" si="19"/>
+        <v>417750</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="18"/>
-        <v>9358</v>
+        <f t="shared" si="20"/>
+        <v>8800</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="19"/>
-        <v>459</v>
+        <f t="shared" si="21"/>
+        <v>600</v>
       </c>
       <c r="J29">
         <v>450</v>
       </c>
       <c r="K29">
-        <f t="shared" si="14"/>
-        <v>578</v>
+        <f t="shared" si="16"/>
+        <v>450</v>
       </c>
       <c r="L29" s="14">
-        <f t="shared" si="15"/>
-        <v>0.62283737024221453</v>
+        <f t="shared" si="17"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="M29">
         <v>15</v>
@@ -7225,7 +7225,7 @@
     </row>
     <row r="30" spans="3:41" x14ac:dyDescent="0.4">
       <c r="C30" s="2">
-        <f t="shared" ref="C30:C54" si="20">C29+1</f>
+        <f t="shared" ref="C30:C54" si="22">C29+1</f>
         <v>26</v>
       </c>
       <c r="D30" s="1">
@@ -7233,34 +7233,34 @@
       </c>
       <c r="E30" s="1">
         <f>542500*(100+$U$7)/100</f>
-        <v>575050</v>
+        <v>542500</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="16"/>
-        <v>74832</v>
+        <f t="shared" si="18"/>
+        <v>70200</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="17"/>
-        <v>520500</v>
+        <f t="shared" si="19"/>
+        <v>487950</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="18"/>
-        <v>10630</v>
+        <f t="shared" si="20"/>
+        <v>10000</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="19"/>
-        <v>813</v>
+        <f t="shared" si="21"/>
+        <v>600</v>
       </c>
       <c r="J30">
         <v>460</v>
       </c>
       <c r="K30">
-        <f t="shared" si="14"/>
-        <v>588</v>
+        <f t="shared" si="16"/>
+        <v>460</v>
       </c>
       <c r="L30" s="14">
-        <f t="shared" si="15"/>
-        <v>0.61224489795918369</v>
+        <f t="shared" si="17"/>
+        <v>0.43478260869565216</v>
       </c>
       <c r="M30">
         <v>16</v>
@@ -7280,7 +7280,7 @@
     </row>
     <row r="31" spans="3:41" x14ac:dyDescent="0.4">
       <c r="C31" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>27</v>
       </c>
       <c r="D31" s="1">
@@ -7288,34 +7288,34 @@
       </c>
       <c r="E31" s="1">
         <f>631600*(100+$U$7)/100</f>
-        <v>669496</v>
+        <v>631600</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="16"/>
-        <v>86746</v>
+        <f t="shared" si="18"/>
+        <v>81400</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="17"/>
-        <v>607246</v>
+        <f t="shared" si="19"/>
+        <v>569350</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="18"/>
-        <v>11914</v>
+        <f t="shared" si="20"/>
+        <v>11200</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="19"/>
-        <v>471</v>
+        <f t="shared" si="21"/>
+        <v>600</v>
       </c>
       <c r="J31">
         <v>470</v>
       </c>
       <c r="K31">
-        <f t="shared" si="14"/>
-        <v>598</v>
+        <f t="shared" si="16"/>
+        <v>470</v>
       </c>
       <c r="L31" s="14">
-        <f t="shared" si="15"/>
-        <v>0.60200668896321075</v>
+        <f t="shared" si="17"/>
+        <v>0.42553191489361702</v>
       </c>
       <c r="M31">
         <v>17</v>
@@ -7335,7 +7335,7 @@
     </row>
     <row r="32" spans="3:41" x14ac:dyDescent="0.4">
       <c r="C32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>28</v>
       </c>
       <c r="D32" s="1">
@@ -7343,34 +7343,34 @@
       </c>
       <c r="E32" s="1">
         <f>733900*(100+$U$7)/100</f>
-        <v>777934</v>
+        <v>733900</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="16"/>
-        <v>100038</v>
+        <f t="shared" si="18"/>
+        <v>93900</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="17"/>
-        <v>707284</v>
+        <f t="shared" si="19"/>
+        <v>663250</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="18"/>
-        <v>13292</v>
+        <f t="shared" si="20"/>
+        <v>12500</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="19"/>
-        <v>907</v>
+        <f t="shared" si="21"/>
+        <v>700</v>
       </c>
       <c r="J32">
         <v>480</v>
       </c>
       <c r="K32">
-        <f t="shared" si="14"/>
-        <v>608</v>
+        <f t="shared" si="16"/>
+        <v>480</v>
       </c>
       <c r="L32" s="14">
-        <f t="shared" si="15"/>
-        <v>0.59210526315789469</v>
+        <f t="shared" si="17"/>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M32">
         <v>18</v>
@@ -7390,7 +7390,7 @@
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C33" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>29</v>
       </c>
       <c r="D33" s="1">
@@ -7398,34 +7398,34 @@
       </c>
       <c r="E33" s="1">
         <f>850900*(100+$U$7)/100</f>
-        <v>901954</v>
+        <v>850900</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="16"/>
-        <v>114820</v>
+        <f t="shared" si="18"/>
+        <v>107800</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="17"/>
-        <v>822104</v>
+        <f t="shared" si="19"/>
+        <v>771050</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="18"/>
-        <v>14782</v>
+        <f t="shared" si="20"/>
+        <v>13900</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="19"/>
-        <v>583</v>
+        <f t="shared" si="21"/>
+        <v>700</v>
       </c>
       <c r="J33">
         <v>490</v>
       </c>
       <c r="K33">
-        <f t="shared" si="14"/>
-        <v>618</v>
+        <f t="shared" si="16"/>
+        <v>490</v>
       </c>
       <c r="L33" s="14">
-        <f t="shared" si="15"/>
-        <v>0.58252427184466016</v>
+        <f t="shared" si="17"/>
+        <v>0.40816326530612246</v>
       </c>
       <c r="M33">
         <v>19</v>
@@ -7445,7 +7445,7 @@
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>30</v>
       </c>
       <c r="D34" s="1">
@@ -7453,34 +7453,34 @@
       </c>
       <c r="E34" s="1">
         <f>984000*(100+$U$7)/100</f>
-        <v>1043040</v>
+        <v>984000</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="16"/>
-        <v>131086</v>
+        <f t="shared" si="18"/>
+        <v>123100</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="17"/>
-        <v>953190</v>
+        <f t="shared" si="19"/>
+        <v>894150</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="18"/>
-        <v>16266</v>
+        <f t="shared" si="20"/>
+        <v>15300</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="19"/>
-        <v>901</v>
+        <f t="shared" si="21"/>
+        <v>700</v>
       </c>
       <c r="J34">
         <v>500</v>
       </c>
       <c r="K34">
-        <f t="shared" si="14"/>
-        <v>628</v>
+        <f t="shared" si="16"/>
+        <v>500</v>
       </c>
       <c r="L34" s="14">
-        <f t="shared" si="15"/>
-        <v>0.57324840764331209</v>
+        <f t="shared" si="17"/>
+        <v>0.4</v>
       </c>
       <c r="M34" s="10">
         <v>20</v>
@@ -7500,7 +7500,7 @@
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C35" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>31</v>
       </c>
       <c r="D35" s="1">
@@ -7508,34 +7508,34 @@
       </c>
       <c r="E35" s="1">
         <f>1134700*(100+$U$7)/100</f>
-        <v>1202782</v>
+        <v>1134700</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="16"/>
-        <v>148942</v>
+        <f t="shared" si="18"/>
+        <v>139900</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="17"/>
-        <v>1102132</v>
+        <f t="shared" si="19"/>
+        <v>1034050</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="18"/>
-        <v>17856</v>
+        <f t="shared" si="20"/>
+        <v>16800</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="19"/>
-        <v>689</v>
+        <f t="shared" si="21"/>
+        <v>800</v>
       </c>
       <c r="J35">
         <v>510</v>
       </c>
       <c r="K35">
-        <f t="shared" si="14"/>
-        <v>638</v>
+        <f t="shared" si="16"/>
+        <v>510</v>
       </c>
       <c r="L35" s="14">
-        <f t="shared" si="15"/>
-        <v>0.56426332288401249</v>
+        <f t="shared" si="17"/>
+        <v>0.39215686274509803</v>
       </c>
       <c r="M35">
         <v>22</v>
@@ -7555,7 +7555,7 @@
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C36" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>32</v>
       </c>
       <c r="D36" s="1">
@@ -7563,34 +7563,34 @@
       </c>
       <c r="E36" s="1">
         <f>1304600*(100+$U$7)/100</f>
-        <v>1382876</v>
+        <v>1304600</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="16"/>
-        <v>168494</v>
+        <f t="shared" si="18"/>
+        <v>158300</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" si="17"/>
-        <v>1270626</v>
+        <f t="shared" si="19"/>
+        <v>1192350</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="18"/>
-        <v>19552</v>
+        <f t="shared" si="20"/>
+        <v>18400</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="19"/>
-        <v>1007</v>
+        <f t="shared" si="21"/>
+        <v>800</v>
       </c>
       <c r="J36">
         <v>520</v>
       </c>
       <c r="K36">
-        <f t="shared" si="14"/>
-        <v>648</v>
+        <f t="shared" si="16"/>
+        <v>520</v>
       </c>
       <c r="L36" s="14">
-        <f t="shared" si="15"/>
-        <v>0.55555555555555558</v>
+        <f t="shared" si="17"/>
+        <v>0.38461538461538464</v>
       </c>
       <c r="M36">
         <v>24</v>
@@ -7610,7 +7610,7 @@
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C37" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>33</v>
       </c>
       <c r="D37" s="1">
@@ -7618,54 +7618,54 @@
       </c>
       <c r="E37" s="1">
         <f>1495400*(100+$U$7)/100</f>
-        <v>1585124</v>
+        <v>1495400</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="16"/>
-        <v>189748</v>
+        <f t="shared" si="18"/>
+        <v>178300</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="17"/>
-        <v>1460374</v>
+        <f t="shared" si="19"/>
+        <v>1370650</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="18"/>
-        <v>21254</v>
+        <f t="shared" si="20"/>
+        <v>20000</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="19"/>
-        <v>695</v>
+        <f t="shared" si="21"/>
+        <v>800</v>
       </c>
       <c r="J37">
         <v>530</v>
       </c>
       <c r="K37">
-        <f t="shared" si="14"/>
-        <v>658</v>
+        <f t="shared" si="16"/>
+        <v>530</v>
       </c>
       <c r="L37" s="14">
-        <f t="shared" si="15"/>
-        <v>0.54711246200607899</v>
+        <f t="shared" si="17"/>
+        <v>0.37735849056603776</v>
       </c>
       <c r="M37">
         <v>26</v>
       </c>
       <c r="N37">
-        <f t="shared" ref="N37:N54" si="21">$M37+$N36</f>
+        <f t="shared" ref="N37:N54" si="23">$M37+$N36</f>
         <v>295.3</v>
       </c>
       <c r="O37">
-        <f t="shared" ref="O37:O54" si="22">$C37*$C37/5</f>
+        <f t="shared" ref="O37:O54" si="24">$C37*$C37/5</f>
         <v>217.8</v>
       </c>
       <c r="P37">
-        <f t="shared" ref="P37:P54" si="23">$O37-O36</f>
+        <f t="shared" ref="P37:P54" si="25">$O37-O36</f>
         <v>13</v>
       </c>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C38" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>34</v>
       </c>
       <c r="D38" s="1">
@@ -7673,54 +7673,54 @@
       </c>
       <c r="E38" s="1">
         <f>1708800*(100+$U$7)/100</f>
-        <v>1811328</v>
+        <v>1708800</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="16"/>
-        <v>212804</v>
+        <f t="shared" si="18"/>
+        <v>200000</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="17"/>
-        <v>1673178</v>
+        <f t="shared" si="19"/>
+        <v>1570650</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="18"/>
-        <v>23056</v>
+        <f t="shared" si="20"/>
+        <v>21700</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="19"/>
-        <v>1107</v>
+        <f t="shared" si="21"/>
+        <v>900</v>
       </c>
       <c r="J38">
         <v>540</v>
       </c>
       <c r="K38">
-        <f t="shared" si="14"/>
-        <v>668</v>
+        <f t="shared" si="16"/>
+        <v>540</v>
       </c>
       <c r="L38" s="14">
-        <f t="shared" si="15"/>
-        <v>0.53892215568862278</v>
+        <f t="shared" si="17"/>
+        <v>0.37037037037037035</v>
       </c>
       <c r="M38">
         <v>28</v>
       </c>
       <c r="N38">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>323.3</v>
       </c>
       <c r="O38">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>231.2</v>
       </c>
       <c r="P38">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>13.399999999999977</v>
       </c>
     </row>
     <row r="39" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C39" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>35</v>
       </c>
       <c r="D39" s="1">
@@ -7728,54 +7728,54 @@
       </c>
       <c r="E39" s="1">
         <f>1946600*(100+$U$7)/100</f>
-        <v>2063396</v>
+        <v>1946600</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="16"/>
-        <v>237768</v>
+        <f t="shared" si="18"/>
+        <v>223500</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="17"/>
-        <v>1910946</v>
+        <f t="shared" si="19"/>
+        <v>1794150</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="18"/>
-        <v>24964</v>
+        <f t="shared" si="20"/>
+        <v>23500</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="19"/>
-        <v>801</v>
+        <f t="shared" si="21"/>
+        <v>900</v>
       </c>
       <c r="J39">
         <v>550</v>
       </c>
       <c r="K39">
-        <f t="shared" si="14"/>
-        <v>678</v>
+        <f t="shared" si="16"/>
+        <v>550</v>
       </c>
       <c r="L39" s="14">
-        <f t="shared" si="15"/>
-        <v>0.53097345132743368</v>
+        <f t="shared" si="17"/>
+        <v>0.36363636363636365</v>
       </c>
       <c r="M39">
         <v>30</v>
       </c>
       <c r="N39">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>353.3</v>
       </c>
       <c r="O39">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>245</v>
       </c>
       <c r="P39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>13.800000000000011</v>
       </c>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C40" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>36</v>
       </c>
       <c r="D40" s="1">
@@ -7783,54 +7783,54 @@
       </c>
       <c r="E40" s="1">
         <f>2210700*(100+$U$7)/100</f>
-        <v>2343342</v>
+        <v>2210700</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" si="16"/>
-        <v>264646</v>
+        <f t="shared" si="18"/>
+        <v>248800</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="17"/>
-        <v>2175592</v>
+        <f t="shared" si="19"/>
+        <v>2042950</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="18"/>
-        <v>26878</v>
+        <f t="shared" si="20"/>
+        <v>25300</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" si="19"/>
-        <v>1113</v>
+        <f t="shared" si="21"/>
+        <v>900</v>
       </c>
       <c r="J40">
         <v>560</v>
       </c>
       <c r="K40">
-        <f t="shared" si="14"/>
-        <v>688</v>
+        <f t="shared" si="16"/>
+        <v>560</v>
       </c>
       <c r="L40" s="14">
-        <f t="shared" si="15"/>
-        <v>0.52325581395348841</v>
+        <f t="shared" si="17"/>
+        <v>0.35714285714285715</v>
       </c>
       <c r="M40">
         <v>32</v>
       </c>
       <c r="N40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>385.3</v>
       </c>
       <c r="O40">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>259.2</v>
       </c>
       <c r="P40">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>14.199999999999989</v>
       </c>
     </row>
     <row r="41" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C41" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>37</v>
       </c>
       <c r="D41" s="1">
@@ -7838,54 +7838,54 @@
       </c>
       <c r="E41" s="1">
         <f>2503000*(100+$U$7)/100</f>
-        <v>2653180</v>
+        <v>2503000</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" si="16"/>
-        <v>293538</v>
+        <f t="shared" si="18"/>
+        <v>276000</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" si="17"/>
-        <v>2469130</v>
+        <f t="shared" si="19"/>
+        <v>2318950</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="18"/>
-        <v>28892</v>
+        <f t="shared" si="20"/>
+        <v>27200</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="19"/>
-        <v>901</v>
+        <f t="shared" si="21"/>
+        <v>1000</v>
       </c>
       <c r="J41">
         <v>570</v>
       </c>
       <c r="K41">
-        <f t="shared" si="14"/>
-        <v>698</v>
+        <f t="shared" si="16"/>
+        <v>570</v>
       </c>
       <c r="L41" s="14">
-        <f t="shared" si="15"/>
-        <v>0.51575931232091687</v>
+        <f t="shared" si="17"/>
+        <v>0.35087719298245612</v>
       </c>
       <c r="M41">
         <v>34</v>
       </c>
       <c r="N41">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>419.3</v>
       </c>
       <c r="O41">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>273.8</v>
       </c>
       <c r="P41">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>14.600000000000023</v>
       </c>
     </row>
     <row r="42" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C42" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>38</v>
       </c>
       <c r="D42" s="1">
@@ -7893,54 +7893,54 @@
       </c>
       <c r="E42" s="1">
         <f>2825500*(100+$U$7)/100</f>
-        <v>2995030</v>
+        <v>2825500</v>
       </c>
       <c r="F42" s="1">
-        <f t="shared" si="16"/>
-        <v>324550</v>
+        <f t="shared" si="18"/>
+        <v>305200</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" si="17"/>
-        <v>2793680</v>
+        <f t="shared" si="19"/>
+        <v>2624150</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="18"/>
-        <v>31012</v>
+        <f t="shared" si="20"/>
+        <v>29200</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" si="19"/>
-        <v>1219</v>
+        <f t="shared" si="21"/>
+        <v>1000</v>
       </c>
       <c r="J42">
         <v>580</v>
       </c>
       <c r="K42">
-        <f t="shared" si="14"/>
-        <v>708</v>
+        <f t="shared" si="16"/>
+        <v>580</v>
       </c>
       <c r="L42" s="14">
-        <f t="shared" si="15"/>
-        <v>0.50847457627118642</v>
+        <f t="shared" si="17"/>
+        <v>0.34482758620689657</v>
       </c>
       <c r="M42">
         <v>36</v>
       </c>
       <c r="N42">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>455.3</v>
       </c>
       <c r="O42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>288.8</v>
       </c>
       <c r="P42">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C43" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>39</v>
       </c>
       <c r="D43" s="1">
@@ -7948,54 +7948,54 @@
       </c>
       <c r="E43" s="1">
         <f>3180300*(100+$U$7)/100</f>
-        <v>3371118</v>
+        <v>3180300</v>
       </c>
       <c r="F43" s="1">
-        <f t="shared" si="16"/>
-        <v>357688</v>
+        <f t="shared" si="18"/>
+        <v>336400</v>
       </c>
       <c r="G43" s="1">
-        <f t="shared" si="17"/>
-        <v>3151368</v>
+        <f t="shared" si="19"/>
+        <v>2960550</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="18"/>
-        <v>33138</v>
+        <f t="shared" si="20"/>
+        <v>31200</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" si="19"/>
-        <v>907</v>
+        <f t="shared" si="21"/>
+        <v>1000</v>
       </c>
       <c r="J43">
         <v>590</v>
       </c>
       <c r="K43">
-        <f t="shared" si="14"/>
-        <v>718</v>
+        <f t="shared" si="16"/>
+        <v>590</v>
       </c>
       <c r="L43" s="14">
-        <f t="shared" si="15"/>
-        <v>0.50139275766016711</v>
+        <f t="shared" si="17"/>
+        <v>0.33898305084745761</v>
       </c>
       <c r="M43">
         <v>38</v>
       </c>
       <c r="N43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>493.3</v>
       </c>
       <c r="O43">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>304.2</v>
       </c>
       <c r="P43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>15.399999999999977</v>
       </c>
     </row>
     <row r="44" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C44" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>40</v>
       </c>
       <c r="D44" s="6">
@@ -8029,21 +8029,21 @@
         <v>50</v>
       </c>
       <c r="N44">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>543.29999999999995</v>
       </c>
       <c r="O44">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>320</v>
       </c>
       <c r="P44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>15.800000000000011</v>
       </c>
     </row>
     <row r="45" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C45" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>41</v>
       </c>
       <c r="D45" s="1">
@@ -8051,19 +8051,19 @@
       </c>
       <c r="E45" s="1">
         <f>3800000*(100+$U$7)/100</f>
-        <v>4028000</v>
+        <v>3800000</v>
       </c>
       <c r="F45" s="1">
         <f>E45-D43-E43</f>
-        <v>637382</v>
+        <v>600200</v>
       </c>
       <c r="G45" s="1">
         <f>F45+G43</f>
-        <v>3788750</v>
+        <v>3560750</v>
       </c>
       <c r="H45" s="1">
         <f>F45-F43</f>
-        <v>279694</v>
+        <v>263800</v>
       </c>
       <c r="I45" s="1">
         <v>0</v>
@@ -8072,32 +8072,32 @@
         <v>620</v>
       </c>
       <c r="K45">
-        <f t="shared" ref="K45:K54" si="24">$J45-$S$7+$R$7</f>
-        <v>748</v>
+        <f t="shared" ref="K45:K54" si="26">$J45-$S$7+$R$7</f>
+        <v>620</v>
       </c>
       <c r="L45" s="14">
-        <f t="shared" ref="L45:L54" si="25">IF($R$4+$R$7&gt;=$K45,100%,($R$4+$R$7)/$K45)</f>
-        <v>0.48128342245989303</v>
+        <f t="shared" ref="L45:L54" si="27">IF($R$4+$R$7&gt;=$K45,100%,($R$4+$R$7)/$K45)</f>
+        <v>0.32258064516129031</v>
       </c>
       <c r="M45">
         <v>55</v>
       </c>
       <c r="N45">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>598.29999999999995</v>
       </c>
       <c r="O45">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>336.2</v>
       </c>
       <c r="P45">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>16.199999999999989</v>
       </c>
     </row>
     <row r="46" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C46" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>42</v>
       </c>
       <c r="D46" s="1">
@@ -8105,54 +8105,54 @@
       </c>
       <c r="E46" s="1">
         <f>4200100*(100+$U$7)/100</f>
-        <v>4452106</v>
+        <v>4200100</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" ref="F46:F54" si="26">E46-D45-E45</f>
-        <v>394106</v>
+        <f t="shared" ref="F46:F54" si="28">E46-D45-E45</f>
+        <v>370100</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" ref="G46:G54" si="27">F46+G45</f>
-        <v>4182856</v>
+        <f t="shared" ref="G46:G54" si="29">F46+G45</f>
+        <v>3930850</v>
       </c>
       <c r="H46" s="1">
         <f>F46-F43</f>
-        <v>36418</v>
+        <v>33700</v>
       </c>
       <c r="I46" s="1">
         <f>H46-H43-I43</f>
-        <v>2373</v>
+        <v>1500</v>
       </c>
       <c r="J46">
         <v>640</v>
       </c>
       <c r="K46">
-        <f t="shared" si="24"/>
-        <v>768</v>
+        <f t="shared" si="26"/>
+        <v>640</v>
       </c>
       <c r="L46" s="14">
-        <f t="shared" si="25"/>
-        <v>0.46875</v>
+        <f t="shared" si="27"/>
+        <v>0.3125</v>
       </c>
       <c r="M46">
         <v>60</v>
       </c>
       <c r="N46">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>658.3</v>
       </c>
       <c r="O46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>352.8</v>
       </c>
       <c r="P46">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>16.600000000000023</v>
       </c>
     </row>
     <row r="47" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C47" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>43</v>
       </c>
       <c r="D47" s="1">
@@ -8160,54 +8160,54 @@
       </c>
       <c r="E47" s="1">
         <f>4640000*(100+$U$7)/100</f>
-        <v>4918400</v>
+        <v>4640000</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" si="26"/>
-        <v>433294</v>
+        <f t="shared" si="28"/>
+        <v>406900</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="27"/>
-        <v>4616150</v>
+        <f t="shared" si="29"/>
+        <v>4337750</v>
       </c>
       <c r="H47" s="1">
-        <f t="shared" ref="H47:H54" si="28">F47-F46</f>
-        <v>39188</v>
+        <f t="shared" ref="H47:H54" si="30">F47-F46</f>
+        <v>36800</v>
       </c>
       <c r="I47" s="1">
         <f>H47-H46-I46</f>
-        <v>397</v>
+        <v>1600</v>
       </c>
       <c r="J47">
         <v>660</v>
       </c>
       <c r="K47">
-        <f t="shared" si="24"/>
-        <v>788</v>
+        <f t="shared" si="26"/>
+        <v>660</v>
       </c>
       <c r="L47" s="14">
-        <f t="shared" si="25"/>
-        <v>0.45685279187817257</v>
+        <f t="shared" si="27"/>
+        <v>0.30303030303030304</v>
       </c>
       <c r="M47">
         <v>65</v>
       </c>
       <c r="N47">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>723.3</v>
       </c>
       <c r="O47">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>369.8</v>
       </c>
       <c r="P47">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>17</v>
       </c>
     </row>
     <row r="48" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C48" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>44</v>
       </c>
       <c r="D48" s="1">
@@ -8215,54 +8215,54 @@
       </c>
       <c r="E48" s="1">
         <f>5123000*(100+$U$7)/100</f>
-        <v>5430380</v>
+        <v>5123000</v>
       </c>
       <c r="F48" s="1">
-        <f t="shared" si="26"/>
-        <v>475980</v>
+        <f t="shared" si="28"/>
+        <v>447000</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" si="27"/>
-        <v>5092130</v>
+        <f t="shared" si="29"/>
+        <v>4784750</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="28"/>
-        <v>42686</v>
+        <f t="shared" si="30"/>
+        <v>40100</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" ref="I48:I54" si="29">H48-H47-I47</f>
-        <v>3101</v>
+        <f t="shared" ref="I48:I54" si="31">H48-H47-I47</f>
+        <v>1700</v>
       </c>
       <c r="J48">
         <v>680</v>
       </c>
       <c r="K48">
-        <f t="shared" si="24"/>
-        <v>808</v>
+        <f t="shared" si="26"/>
+        <v>680</v>
       </c>
       <c r="L48" s="14">
-        <f t="shared" si="25"/>
-        <v>0.44554455445544555</v>
+        <f t="shared" si="27"/>
+        <v>0.29411764705882354</v>
       </c>
       <c r="M48">
         <v>70</v>
       </c>
       <c r="N48">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>793.3</v>
       </c>
       <c r="O48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>387.2</v>
       </c>
       <c r="P48">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>17.399999999999977</v>
       </c>
     </row>
     <row r="49" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C49" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>45</v>
       </c>
       <c r="D49" s="1">
@@ -8270,54 +8270,54 @@
       </c>
       <c r="E49" s="1">
         <f>5652600*(100+$U$7)/100</f>
-        <v>5991756</v>
+        <v>5652600</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" si="26"/>
-        <v>522376</v>
+        <f t="shared" si="28"/>
+        <v>490600</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="27"/>
-        <v>5614506</v>
+        <f t="shared" si="29"/>
+        <v>5275350</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="28"/>
-        <v>46396</v>
+        <f t="shared" si="30"/>
+        <v>43600</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="29"/>
-        <v>609</v>
+        <f t="shared" si="31"/>
+        <v>1800</v>
       </c>
       <c r="J49">
         <v>700</v>
       </c>
       <c r="K49">
-        <f t="shared" si="24"/>
-        <v>828</v>
+        <f t="shared" si="26"/>
+        <v>700</v>
       </c>
       <c r="L49" s="14">
-        <f t="shared" si="25"/>
-        <v>0.43478260869565216</v>
+        <f t="shared" si="27"/>
+        <v>0.2857142857142857</v>
       </c>
       <c r="M49">
         <v>75</v>
       </c>
       <c r="N49">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>868.3</v>
       </c>
       <c r="O49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>405</v>
       </c>
       <c r="P49">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>17.800000000000011</v>
       </c>
     </row>
     <row r="50" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C50" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>46</v>
       </c>
       <c r="D50" s="1">
@@ -8325,54 +8325,54 @@
       </c>
       <c r="E50" s="1">
         <f>6232500*(100+$U$7)/100</f>
-        <v>6606450</v>
+        <v>6232500</v>
       </c>
       <c r="F50" s="1">
-        <f t="shared" si="26"/>
-        <v>572694</v>
+        <f t="shared" si="28"/>
+        <v>537900</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="27"/>
-        <v>6187200</v>
+        <f t="shared" si="29"/>
+        <v>5813250</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="28"/>
-        <v>50318</v>
+        <f t="shared" si="30"/>
+        <v>47300</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="29"/>
-        <v>3313</v>
+        <f t="shared" si="31"/>
+        <v>1900</v>
       </c>
       <c r="J50">
         <v>720</v>
       </c>
       <c r="K50">
-        <f t="shared" si="24"/>
-        <v>848</v>
+        <f t="shared" si="26"/>
+        <v>720</v>
       </c>
       <c r="L50" s="14">
-        <f t="shared" si="25"/>
-        <v>0.42452830188679247</v>
+        <f t="shared" si="27"/>
+        <v>0.27777777777777779</v>
       </c>
       <c r="M50">
         <v>80</v>
       </c>
       <c r="N50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>948.3</v>
       </c>
       <c r="O50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>423.2</v>
       </c>
       <c r="P50">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>18.199999999999989</v>
       </c>
     </row>
     <row r="51" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C51" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
       <c r="D51" s="1">
@@ -8380,54 +8380,54 @@
       </c>
       <c r="E51" s="1">
         <f>6866600*(100+$U$7)/100</f>
-        <v>7278596</v>
+        <v>6866600</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" si="26"/>
-        <v>627146</v>
+        <f t="shared" si="28"/>
+        <v>589100</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="27"/>
-        <v>6814346</v>
+        <f t="shared" si="29"/>
+        <v>6402350</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="28"/>
-        <v>54452</v>
+        <f t="shared" si="30"/>
+        <v>51200</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="29"/>
-        <v>821</v>
+        <f t="shared" si="31"/>
+        <v>2000</v>
       </c>
       <c r="J51">
         <v>740</v>
       </c>
       <c r="K51">
-        <f t="shared" si="24"/>
-        <v>868</v>
+        <f t="shared" si="26"/>
+        <v>740</v>
       </c>
       <c r="L51" s="14">
-        <f t="shared" si="25"/>
-        <v>0.41474654377880182</v>
+        <f t="shared" si="27"/>
+        <v>0.27027027027027029</v>
       </c>
       <c r="M51">
         <v>85</v>
       </c>
       <c r="N51">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1033.3</v>
       </c>
       <c r="O51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>441.8</v>
       </c>
       <c r="P51">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>18.600000000000023</v>
       </c>
     </row>
     <row r="52" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C52" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
       <c r="D52" s="1">
@@ -8435,54 +8435,54 @@
       </c>
       <c r="E52" s="1">
         <f>7561000*(100+$U$7)/100</f>
-        <v>8014660</v>
+        <v>7561000</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" si="26"/>
-        <v>686064</v>
+        <f t="shared" si="28"/>
+        <v>644400</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="27"/>
-        <v>7500410</v>
+        <f t="shared" si="29"/>
+        <v>7046750</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="28"/>
-        <v>58918</v>
+        <f t="shared" si="30"/>
+        <v>55300</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="29"/>
-        <v>3645</v>
+        <f t="shared" si="31"/>
+        <v>2100</v>
       </c>
       <c r="J52">
         <v>760</v>
       </c>
       <c r="K52">
-        <f t="shared" si="24"/>
-        <v>888</v>
+        <f t="shared" si="26"/>
+        <v>760</v>
       </c>
       <c r="L52" s="14">
-        <f t="shared" si="25"/>
-        <v>0.40540540540540543</v>
+        <f t="shared" si="27"/>
+        <v>0.26315789473684209</v>
       </c>
       <c r="M52">
         <v>90</v>
       </c>
       <c r="N52">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1123.3</v>
       </c>
       <c r="O52">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>460.8</v>
       </c>
       <c r="P52">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>19</v>
       </c>
     </row>
     <row r="53" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C53" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>49</v>
       </c>
       <c r="D53" s="1">
@@ -8490,54 +8490,54 @@
       </c>
       <c r="E53" s="1">
         <f>8320000*(100+$U$7)/100</f>
-        <v>8819200</v>
+        <v>8320000</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" si="26"/>
-        <v>749540</v>
+        <f t="shared" si="28"/>
+        <v>704000</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="27"/>
-        <v>8249950</v>
+        <f t="shared" si="29"/>
+        <v>7750750</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="28"/>
-        <v>63476</v>
+        <f t="shared" si="30"/>
+        <v>59600</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="29"/>
-        <v>913</v>
+        <f t="shared" si="31"/>
+        <v>2200</v>
       </c>
       <c r="J53">
         <v>780</v>
       </c>
       <c r="K53">
-        <f t="shared" si="24"/>
-        <v>908</v>
+        <f t="shared" si="26"/>
+        <v>780</v>
       </c>
       <c r="L53" s="14">
-        <f t="shared" si="25"/>
-        <v>0.3964757709251101</v>
+        <f t="shared" si="27"/>
+        <v>0.25641025641025639</v>
       </c>
       <c r="M53">
         <v>95</v>
       </c>
       <c r="N53">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1218.3</v>
       </c>
       <c r="O53">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>480.2</v>
       </c>
       <c r="P53">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>19.399999999999977</v>
       </c>
     </row>
     <row r="54" spans="3:16" x14ac:dyDescent="0.4">
       <c r="C54" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>50</v>
       </c>
       <c r="D54" s="1">
@@ -8545,48 +8545,48 @@
       </c>
       <c r="E54" s="1">
         <f>9148100*(100+$U$7)/100</f>
-        <v>9696986</v>
+        <v>9148100</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" si="26"/>
-        <v>817786</v>
+        <f t="shared" si="28"/>
+        <v>768100</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="27"/>
-        <v>9067736</v>
+        <f t="shared" si="29"/>
+        <v>8518850</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="28"/>
-        <v>68246</v>
+        <f t="shared" si="30"/>
+        <v>64100</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="29"/>
-        <v>3857</v>
+        <f t="shared" si="31"/>
+        <v>2300</v>
       </c>
       <c r="J54">
         <v>800</v>
       </c>
       <c r="K54">
-        <f t="shared" si="24"/>
-        <v>928</v>
+        <f t="shared" si="26"/>
+        <v>800</v>
       </c>
       <c r="L54" s="14">
-        <f t="shared" si="25"/>
-        <v>0.38793103448275862</v>
+        <f t="shared" si="27"/>
+        <v>0.25</v>
       </c>
       <c r="M54" s="10">
         <v>100</v>
       </c>
       <c r="N54">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1318.3</v>
       </c>
       <c r="O54">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>500</v>
       </c>
       <c r="P54">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>19.800000000000011</v>
       </c>
     </row>

</xml_diff>